<commit_message>
Modificato report-checklist.xlsx - V2
09/05/2023
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ADSFINMATIC/Data_Processing_SPA/SmartHealth/4.5.048/report-checklist.xlsx
+++ b/GATEWAY/A1#111ADSFINMATIC/Data_Processing_SPA/SmartHealth/4.5.048/report-checklist.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="462">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2120,6 +2120,9 @@
   </si>
   <si>
     <t>I modelli di LDO prevedono solo sezione 'terapie farmacologiche alla dimissione' di tipo testuale, non viene gestita alcuna Entry</t>
+  </si>
+  <si>
+    <t>In questa fase, in cui non è necessaria la firma digitale dei documenti, quelli per cui l'invio fallisce vengono riportati in stato NON validato per essere disponibili a nuova validazione ed invio : viene data evidenza dei documenti in questo stato.</t>
   </si>
 </sst>
 </file>
@@ -2903,7 +2906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4081,10 +4084,10 @@
   <dimension ref="A1:T746"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B126" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="K52" sqref="K52"/>
+      <selection pane="bottomRight" activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -5087,8 +5090,12 @@
       <c r="N26" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
+      <c r="O26" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P26" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q26" s="24"/>
       <c r="R26" s="25"/>
       <c r="S26" s="26"/>
@@ -5137,8 +5144,12 @@
       <c r="N27" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
+      <c r="O27" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P27" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q27" s="24"/>
       <c r="R27" s="25"/>
       <c r="S27" s="26"/>
@@ -5187,8 +5198,12 @@
       <c r="N28" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
+      <c r="O28" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P28" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q28" s="24"/>
       <c r="R28" s="25"/>
       <c r="S28" s="26"/>
@@ -5237,8 +5252,12 @@
       <c r="N29" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
+      <c r="O29" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P29" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q29" s="24"/>
       <c r="R29" s="25"/>
       <c r="S29" s="26"/>
@@ -5287,8 +5306,12 @@
       <c r="N30" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
+      <c r="O30" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P30" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q30" s="24"/>
       <c r="R30" s="25"/>
       <c r="S30" s="26"/>
@@ -5337,8 +5360,12 @@
       <c r="N31" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
+      <c r="O31" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P31" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q31" s="24"/>
       <c r="R31" s="25"/>
       <c r="S31" s="26"/>
@@ -5387,8 +5414,12 @@
       <c r="N32" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
+      <c r="O32" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P32" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q32" s="24"/>
       <c r="R32" s="25"/>
       <c r="S32" s="26"/>
@@ -5437,8 +5468,12 @@
       <c r="N33" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
+      <c r="O33" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P33" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q33" s="24"/>
       <c r="R33" s="25"/>
       <c r="S33" s="26"/>
@@ -5487,8 +5522,12 @@
       <c r="N34" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
+      <c r="O34" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P34" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q34" s="24"/>
       <c r="R34" s="25"/>
       <c r="S34" s="26"/>
@@ -5537,8 +5576,12 @@
       <c r="N35" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
+      <c r="O35" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P35" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q35" s="24"/>
       <c r="R35" s="25"/>
       <c r="S35" s="26"/>

</xml_diff>

<commit_message>
Cambiato file report-checklist.xlsx - V3
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ADSFINMATIC/Data_Processing_SPA/SmartHealth/4.5.048/report-checklist.xlsx
+++ b/GATEWAY/A1#111ADSFINMATIC/Data_Processing_SPA/SmartHealth/4.5.048/report-checklist.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="463">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1673,9 +1673,6 @@
     <t>I ns modelli di LDO prevedono solo sezione 'terapie farmacologiche alla dimissione' di tipo testuale, non viene gestita alcuna Entry</t>
   </si>
   <si>
-    <t>Errore bloccante a video di timeout dell'operazione</t>
-  </si>
-  <si>
     <t>La composizione del CDA in Applicativo prevede solo la valorizzazione del confidentialityCode con i valori N (Normal) per documenti non oscurati e V (Very restricted) per documenti oscurati</t>
   </si>
   <si>
@@ -2123,12 +2120,20 @@
   </si>
   <si>
     <t>In questa fase, in cui non è necessaria la firma digitale dei documenti, quelli per cui l'invio fallisce vengono riportati in stato NON validato per essere disponibili a nuova validazione ed invio : viene data evidenza dei documenti in questo stato.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Errore bloccante a video di timeout dell'operazione. In questa fase, in cui non è necessaria la firma digitale dei documenti, quelli per cui l'invio fallisce vengono riportati in stato NON validato per essere disponibili a nuova validazione ed invio : viene data evidenza dei documenti in questo stato.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In questa fase, in cui non è necessaria la firma digitale dei documenti, quelli per cui l'invio fallisce vengono riportati in stato NON validato per essere disponibili a nuova validazione ed invio : viene data evidenza dei documenti in questo stato.
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
@@ -2910,10 +2915,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="130.1796875" customWidth="1"/>
-    <col min="2" max="26" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="130.140625" customWidth="1"/>
+    <col min="2" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2921,27 +2926,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="87">
+    <row r="2" spans="1:1" ht="90">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="29">
+    <row r="3" spans="1:1" ht="30">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="174">
+    <row r="4" spans="1:1" ht="195">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="29">
+    <row r="5" spans="1:1" ht="30">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="29">
+    <row r="6" spans="1:1" ht="30">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2959,7 +2964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="29">
+    <row r="10" spans="1:1" ht="45">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2987,11 +2992,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" customWidth="1"/>
-    <col min="2" max="2" width="194.1796875" customWidth="1"/>
-    <col min="3" max="26" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="194.140625" customWidth="1"/>
+    <col min="3" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -3063,7 +3068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="43.5">
+    <row r="11" spans="1:2" ht="45">
       <c r="A11" s="10">
         <v>8</v>
       </c>
@@ -4083,28 +4088,28 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="L96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P32" sqref="P32"/>
+      <selection pane="bottomRight" activeCell="P97" sqref="P97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
-    <col min="2" max="2" width="46.81640625" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" customWidth="1"/>
-    <col min="4" max="4" width="63.81640625" customWidth="1"/>
-    <col min="5" max="5" width="104.81640625" customWidth="1"/>
-    <col min="6" max="9" width="33.1796875" customWidth="1"/>
-    <col min="10" max="10" width="27.1796875" customWidth="1"/>
-    <col min="11" max="15" width="36.453125" customWidth="1"/>
-    <col min="16" max="16" width="27.1796875" customWidth="1"/>
-    <col min="17" max="17" width="33.1796875" customWidth="1"/>
-    <col min="18" max="18" width="36.453125" customWidth="1"/>
-    <col min="19" max="20" width="31.81640625" customWidth="1"/>
-    <col min="21" max="26" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="63.85546875" customWidth="1"/>
+    <col min="5" max="5" width="104.85546875" customWidth="1"/>
+    <col min="6" max="9" width="33.140625" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" customWidth="1"/>
+    <col min="11" max="15" width="36.42578125" customWidth="1"/>
+    <col min="16" max="16" width="27.140625" customWidth="1"/>
+    <col min="17" max="17" width="33.140625" customWidth="1"/>
+    <col min="18" max="18" width="36.42578125" customWidth="1"/>
+    <col min="19" max="20" width="31.85546875" customWidth="1"/>
+    <col min="21" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" customHeight="1">
@@ -4341,7 +4346,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="10" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A10" s="20">
         <v>6</v>
       </c>
@@ -4385,7 +4390,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="11" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A11" s="20">
         <v>7</v>
       </c>
@@ -4408,10 +4413,10 @@
         <v>44985.513518518521</v>
       </c>
       <c r="H11" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="I11" s="36" t="s">
         <v>318</v>
-      </c>
-      <c r="I11" s="36" t="s">
-        <v>319</v>
       </c>
       <c r="J11" s="33" t="s">
         <v>105</v>
@@ -4429,7 +4434,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="12" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A12" s="20">
         <v>8</v>
       </c>
@@ -4452,10 +4457,10 @@
         <v>44986.648530092592</v>
       </c>
       <c r="H12" s="37" t="s">
+        <v>319</v>
+      </c>
+      <c r="I12" s="36" t="s">
         <v>320</v>
-      </c>
-      <c r="I12" s="36" t="s">
-        <v>321</v>
       </c>
       <c r="J12" s="33" t="s">
         <v>105</v>
@@ -4473,7 +4478,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="13" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A13" s="20">
         <v>9</v>
       </c>
@@ -4496,10 +4501,10 @@
         <v>45020.720949074072</v>
       </c>
       <c r="H13" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="I13" s="36" t="s">
         <v>322</v>
-      </c>
-      <c r="I13" s="36" t="s">
-        <v>323</v>
       </c>
       <c r="J13" s="33" t="s">
         <v>105</v>
@@ -4517,7 +4522,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="14" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A14" s="20">
         <v>16</v>
       </c>
@@ -4540,10 +4545,10 @@
         <v>45033.477523148147</v>
       </c>
       <c r="H14" s="38" t="s">
+        <v>323</v>
+      </c>
+      <c r="I14" s="36" t="s">
         <v>324</v>
-      </c>
-      <c r="I14" s="36" t="s">
-        <v>325</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>105</v>
@@ -4561,7 +4566,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="15" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A15" s="20">
         <v>17</v>
       </c>
@@ -4584,10 +4589,10 @@
         <v>45033.721053240741</v>
       </c>
       <c r="H15" s="38" t="s">
+        <v>325</v>
+      </c>
+      <c r="I15" s="36" t="s">
         <v>326</v>
-      </c>
-      <c r="I15" s="36" t="s">
-        <v>327</v>
       </c>
       <c r="J15" s="33" t="s">
         <v>105</v>
@@ -4605,7 +4610,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="16" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A16" s="20">
         <v>18</v>
       </c>
@@ -4628,10 +4633,10 @@
         <v>45034.650752314818</v>
       </c>
       <c r="H16" s="38" t="s">
+        <v>335</v>
+      </c>
+      <c r="I16" s="36" t="s">
         <v>336</v>
-      </c>
-      <c r="I16" s="36" t="s">
-        <v>337</v>
       </c>
       <c r="J16" s="33" t="s">
         <v>105</v>
@@ -4649,7 +4654,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="17" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A17" s="20">
         <v>19</v>
       </c>
@@ -4672,10 +4677,10 @@
         <v>45034.665543981479</v>
       </c>
       <c r="H17" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="I17" s="36" t="s">
         <v>338</v>
-      </c>
-      <c r="I17" s="36" t="s">
-        <v>339</v>
       </c>
       <c r="J17" s="33" t="s">
         <v>105</v>
@@ -4693,7 +4698,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="18" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A18" s="20">
         <v>20</v>
       </c>
@@ -4716,10 +4721,10 @@
         <v>45034.714479166665</v>
       </c>
       <c r="H18" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="I18" s="36" t="s">
         <v>340</v>
-      </c>
-      <c r="I18" s="36" t="s">
-        <v>341</v>
       </c>
       <c r="J18" s="33" t="s">
         <v>105</v>
@@ -4737,7 +4742,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="19" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A19" s="20">
         <v>21</v>
       </c>
@@ -4760,10 +4765,10 @@
         <v>45034.729537037034</v>
       </c>
       <c r="H19" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="I19" s="36" t="s">
         <v>342</v>
-      </c>
-      <c r="I19" s="36" t="s">
-        <v>343</v>
       </c>
       <c r="J19" s="33" t="s">
         <v>105</v>
@@ -4781,7 +4786,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="20" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A20" s="20">
         <v>22</v>
       </c>
@@ -4804,10 +4809,10 @@
         <v>45034.75167824074</v>
       </c>
       <c r="H20" s="38" t="s">
+        <v>343</v>
+      </c>
+      <c r="I20" s="36" t="s">
         <v>344</v>
-      </c>
-      <c r="I20" s="36" t="s">
-        <v>345</v>
       </c>
       <c r="J20" s="33" t="s">
         <v>105</v>
@@ -4825,7 +4830,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="21" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A21" s="20">
         <v>23</v>
       </c>
@@ -4848,10 +4853,10 @@
         <v>45034.762800925928</v>
       </c>
       <c r="H21" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="I21" s="36" t="s">
         <v>346</v>
-      </c>
-      <c r="I21" s="36" t="s">
-        <v>347</v>
       </c>
       <c r="J21" s="33" t="s">
         <v>105</v>
@@ -4869,7 +4874,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="22" spans="1:20" ht="150.75" thickBot="1">
       <c r="A22" s="20">
         <v>24</v>
       </c>
@@ -4892,10 +4897,10 @@
         <v>45015.712592592594</v>
       </c>
       <c r="H22" s="38" t="s">
+        <v>347</v>
+      </c>
+      <c r="I22" s="36" t="s">
         <v>348</v>
-      </c>
-      <c r="I22" s="36" t="s">
-        <v>349</v>
       </c>
       <c r="J22" s="33" t="s">
         <v>105</v>
@@ -4913,7 +4918,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="23" spans="1:20" ht="150.75" thickBot="1">
       <c r="A23" s="20">
         <v>25</v>
       </c>
@@ -4936,10 +4941,10 @@
         <v>45036.656076388892</v>
       </c>
       <c r="H23" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="I23" s="36" t="s">
         <v>350</v>
-      </c>
-      <c r="I23" s="36" t="s">
-        <v>351</v>
       </c>
       <c r="J23" s="33" t="s">
         <v>105</v>
@@ -4957,7 +4962,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="24" spans="1:20" ht="150.75" thickBot="1">
       <c r="A24" s="20">
         <v>26</v>
       </c>
@@ -4980,16 +4985,16 @@
         <v>45037.599317129629</v>
       </c>
       <c r="H24" s="38" t="s">
+        <v>352</v>
+      </c>
+      <c r="I24" s="36" t="s">
         <v>353</v>
-      </c>
-      <c r="I24" s="36" t="s">
-        <v>354</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>302</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
@@ -5003,7 +5008,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="25" spans="1:20" ht="150.75" thickBot="1">
       <c r="A25" s="20">
         <v>27</v>
       </c>
@@ -5026,16 +5031,16 @@
         <v>45037.717083333337</v>
       </c>
       <c r="H25" s="38" t="s">
+        <v>354</v>
+      </c>
+      <c r="I25" s="36" t="s">
         <v>355</v>
-      </c>
-      <c r="I25" s="36" t="s">
-        <v>356</v>
       </c>
       <c r="J25" s="33" t="s">
         <v>302</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
@@ -5049,7 +5054,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="145.5" hidden="1" thickBot="1">
+    <row r="26" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A26" s="20">
         <v>29</v>
       </c>
@@ -5072,10 +5077,10 @@
         <v>45049.443703703706</v>
       </c>
       <c r="H26" s="36" t="s">
+        <v>373</v>
+      </c>
+      <c r="I26" s="36" t="s">
         <v>374</v>
-      </c>
-      <c r="I26" s="36" t="s">
-        <v>375</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>105</v>
@@ -5088,13 +5093,13 @@
         <v>105</v>
       </c>
       <c r="N26" s="24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="O26" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P26" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q26" s="24"/>
       <c r="R26" s="25"/>
@@ -5103,7 +5108,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="145.5" thickBot="1">
+    <row r="27" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A27" s="20">
         <v>32</v>
       </c>
@@ -5126,10 +5131,10 @@
         <v>45051.682210648149</v>
       </c>
       <c r="H27" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>105</v>
@@ -5142,13 +5147,13 @@
         <v>105</v>
       </c>
       <c r="N27" s="24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="O27" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P27" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q27" s="24"/>
       <c r="R27" s="25"/>
@@ -5157,7 +5162,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="145.5" hidden="1" thickBot="1">
+    <row r="28" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A28" s="20">
         <v>33</v>
       </c>
@@ -5180,10 +5185,10 @@
         <v>45049.487303240741</v>
       </c>
       <c r="H28" s="38" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I28" s="36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J28" s="33" t="s">
         <v>105</v>
@@ -5196,13 +5201,13 @@
         <v>105</v>
       </c>
       <c r="N28" s="24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="O28" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P28" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q28" s="24"/>
       <c r="R28" s="25"/>
@@ -5211,7 +5216,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="145.5" hidden="1" thickBot="1">
+    <row r="29" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A29" s="20">
         <v>34</v>
       </c>
@@ -5234,10 +5239,10 @@
         <v>45049.728391203702</v>
       </c>
       <c r="H29" s="38" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I29" s="36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J29" s="33" t="s">
         <v>105</v>
@@ -5250,13 +5255,13 @@
         <v>105</v>
       </c>
       <c r="N29" s="24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="O29" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P29" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q29" s="24"/>
       <c r="R29" s="25"/>
@@ -5265,7 +5270,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="145.5" hidden="1" thickBot="1">
+    <row r="30" spans="1:20" ht="150.75" thickBot="1">
       <c r="A30" s="20">
         <v>35</v>
       </c>
@@ -5288,10 +5293,10 @@
         <v>45050.682233796295</v>
       </c>
       <c r="H30" s="38" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I30" s="36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J30" s="33" t="s">
         <v>105</v>
@@ -5304,13 +5309,13 @@
         <v>105</v>
       </c>
       <c r="N30" s="24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="O30" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P30" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q30" s="24"/>
       <c r="R30" s="25"/>
@@ -5319,7 +5324,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="145.5" hidden="1" thickBot="1">
+    <row r="31" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A31" s="20">
         <v>37</v>
       </c>
@@ -5342,10 +5347,10 @@
         <v>45049.458009259259</v>
       </c>
       <c r="H31" s="38" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I31" s="36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J31" s="33" t="s">
         <v>105</v>
@@ -5358,13 +5363,13 @@
         <v>105</v>
       </c>
       <c r="N31" s="24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O31" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P31" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q31" s="24"/>
       <c r="R31" s="25"/>
@@ -5373,7 +5378,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="145.5" thickBot="1">
+    <row r="32" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A32" s="20">
         <v>40</v>
       </c>
@@ -5396,10 +5401,10 @@
         <v>45051.703449074077</v>
       </c>
       <c r="H32" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I32" s="36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J32" s="33" t="s">
         <v>105</v>
@@ -5412,13 +5417,13 @@
         <v>105</v>
       </c>
       <c r="N32" s="24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O32" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P32" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q32" s="24"/>
       <c r="R32" s="25"/>
@@ -5427,7 +5432,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="145.5" hidden="1" thickBot="1">
+    <row r="33" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A33" s="20">
         <v>41</v>
       </c>
@@ -5450,10 +5455,10 @@
         <v>45049.504143518519</v>
       </c>
       <c r="H33" s="38" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I33" s="36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J33" s="33" t="s">
         <v>105</v>
@@ -5466,13 +5471,13 @@
         <v>105</v>
       </c>
       <c r="N33" s="24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O33" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P33" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q33" s="24"/>
       <c r="R33" s="25"/>
@@ -5481,7 +5486,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="145.5" hidden="1" thickBot="1">
+    <row r="34" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A34" s="20">
         <v>42</v>
       </c>
@@ -5504,10 +5509,10 @@
         <v>45050.45894675926</v>
       </c>
       <c r="H34" s="38" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I34" s="36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>105</v>
@@ -5520,13 +5525,13 @@
         <v>105</v>
       </c>
       <c r="N34" s="24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O34" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P34" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q34" s="24"/>
       <c r="R34" s="25"/>
@@ -5535,7 +5540,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="145.5" hidden="1" thickBot="1">
+    <row r="35" spans="1:20" ht="165.75" thickBot="1">
       <c r="A35" s="20">
         <v>43</v>
       </c>
@@ -5558,10 +5563,10 @@
         <v>45050.726701388892</v>
       </c>
       <c r="H35" s="38" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I35" s="36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J35" s="33" t="s">
         <v>105</v>
@@ -5574,13 +5579,13 @@
         <v>105</v>
       </c>
       <c r="N35" s="24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O35" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P35" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Q35" s="24"/>
       <c r="R35" s="25"/>
@@ -5589,7 +5594,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="44" hidden="1" thickBot="1">
+    <row r="36" spans="1:20" ht="195.75" hidden="1" thickBot="1">
       <c r="A36" s="20">
         <v>45</v>
       </c>
@@ -5609,17 +5614,15 @@
       <c r="G36" s="35"/>
       <c r="H36" s="38"/>
       <c r="I36" s="36"/>
-      <c r="J36" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="K36" s="24" t="s">
-        <v>312</v>
-      </c>
+      <c r="J36" s="33"/>
+      <c r="K36" s="24"/>
       <c r="L36" s="24"/>
       <c r="M36" s="24"/>
       <c r="N36" s="24"/>
       <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
+      <c r="P36" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q36" s="24"/>
       <c r="R36" s="25" t="s">
         <v>105</v>
@@ -5629,7 +5632,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="44" thickBot="1">
+    <row r="37" spans="1:20" ht="195.75" hidden="1" thickBot="1">
       <c r="A37" s="20">
         <v>48</v>
       </c>
@@ -5649,17 +5652,15 @@
       <c r="G37" s="35"/>
       <c r="H37" s="38"/>
       <c r="I37" s="36"/>
-      <c r="J37" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="K37" s="24" t="s">
-        <v>312</v>
-      </c>
+      <c r="J37" s="33"/>
+      <c r="K37" s="24"/>
       <c r="L37" s="24"/>
       <c r="M37" s="24"/>
       <c r="N37" s="24"/>
       <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
+      <c r="P37" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q37" s="24"/>
       <c r="R37" s="25" t="s">
         <v>105</v>
@@ -5669,7 +5670,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="44" hidden="1" thickBot="1">
+    <row r="38" spans="1:20" ht="195.75" hidden="1" thickBot="1">
       <c r="A38" s="20">
         <v>49</v>
       </c>
@@ -5689,17 +5690,15 @@
       <c r="G38" s="35"/>
       <c r="H38" s="38"/>
       <c r="I38" s="36"/>
-      <c r="J38" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="K38" s="24" t="s">
-        <v>312</v>
-      </c>
+      <c r="J38" s="33"/>
+      <c r="K38" s="24"/>
       <c r="L38" s="24"/>
       <c r="M38" s="24"/>
       <c r="N38" s="24"/>
       <c r="O38" s="24"/>
-      <c r="P38" s="24"/>
+      <c r="P38" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q38" s="24"/>
       <c r="R38" s="25" t="s">
         <v>105</v>
@@ -5709,7 +5708,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="44" hidden="1" thickBot="1">
+    <row r="39" spans="1:20" ht="195.75" hidden="1" thickBot="1">
       <c r="A39" s="20">
         <v>50</v>
       </c>
@@ -5729,17 +5728,15 @@
       <c r="G39" s="35"/>
       <c r="H39" s="38"/>
       <c r="I39" s="36"/>
-      <c r="J39" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="K39" s="24" t="s">
-        <v>312</v>
-      </c>
+      <c r="J39" s="33"/>
+      <c r="K39" s="24"/>
       <c r="L39" s="24"/>
       <c r="M39" s="24"/>
       <c r="N39" s="24"/>
       <c r="O39" s="24"/>
-      <c r="P39" s="24"/>
+      <c r="P39" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q39" s="24"/>
       <c r="R39" s="25" t="s">
         <v>105</v>
@@ -5749,7 +5746,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="44" hidden="1" thickBot="1">
+    <row r="40" spans="1:20" ht="195.75" thickBot="1">
       <c r="A40" s="20">
         <v>51</v>
       </c>
@@ -5769,17 +5766,15 @@
       <c r="G40" s="35"/>
       <c r="H40" s="38"/>
       <c r="I40" s="36"/>
-      <c r="J40" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="K40" s="24" t="s">
-        <v>312</v>
-      </c>
+      <c r="J40" s="33"/>
+      <c r="K40" s="24"/>
       <c r="L40" s="24"/>
       <c r="M40" s="24"/>
       <c r="N40" s="24"/>
       <c r="O40" s="24"/>
-      <c r="P40" s="24"/>
+      <c r="P40" s="24" t="s">
+        <v>461</v>
+      </c>
       <c r="Q40" s="24"/>
       <c r="R40" s="25" t="s">
         <v>105</v>
@@ -5789,7 +5784,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="41" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A41" s="20">
         <v>63</v>
       </c>
@@ -5812,13 +5807,13 @@
         <v>45048.703414351854</v>
       </c>
       <c r="H41" s="38" t="s">
+        <v>370</v>
+      </c>
+      <c r="I41" s="36" t="s">
         <v>371</v>
       </c>
-      <c r="I41" s="36" t="s">
-        <v>372</v>
-      </c>
       <c r="J41" s="33" t="s">
-        <v>302</v>
+        <v>105</v>
       </c>
       <c r="K41" s="33"/>
       <c r="L41" s="24" t="s">
@@ -5828,10 +5823,14 @@
         <v>105</v>
       </c>
       <c r="N41" s="24" t="s">
-        <v>373</v>
-      </c>
-      <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
+        <v>372</v>
+      </c>
+      <c r="O41" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P41" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q41" s="24"/>
       <c r="R41" s="25"/>
       <c r="S41" s="26"/>
@@ -5839,7 +5838,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="42" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A42" s="20">
         <v>64</v>
       </c>
@@ -5863,7 +5862,7 @@
         <v>302</v>
       </c>
       <c r="K42" s="33" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L42" s="24"/>
       <c r="M42" s="24"/>
@@ -5877,7 +5876,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="43" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A43" s="20">
         <v>65</v>
       </c>
@@ -5901,7 +5900,7 @@
         <v>302</v>
       </c>
       <c r="K43" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L43" s="24"/>
       <c r="M43" s="24"/>
@@ -5915,7 +5914,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="44" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A44" s="20">
         <v>66</v>
       </c>
@@ -5953,7 +5952,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="45" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A45" s="20">
         <v>67</v>
       </c>
@@ -5991,7 +5990,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="46" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A46" s="20">
         <v>68</v>
       </c>
@@ -6015,7 +6014,7 @@
         <v>302</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L46" s="24"/>
       <c r="M46" s="24"/>
@@ -6029,7 +6028,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="47" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A47" s="20">
         <v>69</v>
       </c>
@@ -6053,7 +6052,7 @@
         <v>302</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="L47" s="24"/>
       <c r="M47" s="24"/>
@@ -6067,7 +6066,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="48" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A48" s="20">
         <v>70</v>
       </c>
@@ -6091,7 +6090,7 @@
         <v>302</v>
       </c>
       <c r="K48" s="33" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L48" s="24"/>
       <c r="M48" s="24"/>
@@ -6105,7 +6104,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="49" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A49" s="20">
         <v>71</v>
       </c>
@@ -6129,7 +6128,7 @@
         <v>302</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L49" s="24"/>
       <c r="M49" s="24"/>
@@ -6143,7 +6142,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="50" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A50" s="20">
         <v>72</v>
       </c>
@@ -6181,7 +6180,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="51" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A51" s="20">
         <v>73</v>
       </c>
@@ -6204,10 +6203,10 @@
         <v>45048.681261574071</v>
       </c>
       <c r="H51" s="38" t="s">
+        <v>367</v>
+      </c>
+      <c r="I51" s="36" t="s">
         <v>368</v>
-      </c>
-      <c r="I51" s="36" t="s">
-        <v>369</v>
       </c>
       <c r="J51" s="33" t="s">
         <v>105</v>
@@ -6220,10 +6219,14 @@
         <v>105</v>
       </c>
       <c r="N51" s="24" t="s">
-        <v>370</v>
-      </c>
-      <c r="O51" s="24"/>
-      <c r="P51" s="24"/>
+        <v>369</v>
+      </c>
+      <c r="O51" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P51" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q51" s="24"/>
       <c r="R51" s="25"/>
       <c r="S51" s="26"/>
@@ -6231,7 +6234,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="52" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A52" s="20">
         <v>74</v>
       </c>
@@ -6255,7 +6258,7 @@
         <v>302</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="L52" s="24"/>
       <c r="M52" s="24"/>
@@ -6269,7 +6272,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="53" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A53" s="20">
         <v>94</v>
       </c>
@@ -6293,7 +6296,7 @@
         <v>302</v>
       </c>
       <c r="K53" s="24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L53" s="24"/>
       <c r="M53" s="24"/>
@@ -6307,7 +6310,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="54" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A54" s="20">
         <v>95</v>
       </c>
@@ -6331,7 +6334,7 @@
         <v>302</v>
       </c>
       <c r="K54" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L54" s="24"/>
       <c r="M54" s="24"/>
@@ -6345,7 +6348,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="55" spans="1:20" ht="105.75" hidden="1" thickBot="1">
       <c r="A55" s="20">
         <v>96</v>
       </c>
@@ -6369,7 +6372,7 @@
         <v>302</v>
       </c>
       <c r="K55" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L55" s="24"/>
       <c r="M55" s="24"/>
@@ -6383,7 +6386,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="56" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A56" s="20">
         <v>97</v>
       </c>
@@ -6421,7 +6424,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="57" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A57" s="20">
         <v>98</v>
       </c>
@@ -6459,7 +6462,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="58" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A58" s="20">
         <v>99</v>
       </c>
@@ -6483,7 +6486,7 @@
         <v>302</v>
       </c>
       <c r="K58" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L58" s="24"/>
       <c r="M58" s="24"/>
@@ -6497,7 +6500,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="59" spans="1:20" ht="105.75" hidden="1" thickBot="1">
       <c r="A59" s="20">
         <v>100</v>
       </c>
@@ -6521,7 +6524,7 @@
         <v>302</v>
       </c>
       <c r="K59" s="24" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L59" s="24"/>
       <c r="M59" s="24"/>
@@ -6535,7 +6538,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="60" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A60" s="20">
         <v>101</v>
       </c>
@@ -6559,7 +6562,7 @@
         <v>302</v>
       </c>
       <c r="K60" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L60" s="24"/>
       <c r="M60" s="24"/>
@@ -6573,7 +6576,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="61" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A61" s="20">
         <v>102</v>
       </c>
@@ -6596,10 +6599,10 @@
         <v>45049.579837962963</v>
       </c>
       <c r="H61" s="38" t="s">
+        <v>380</v>
+      </c>
+      <c r="I61" s="36" t="s">
         <v>381</v>
-      </c>
-      <c r="I61" s="36" t="s">
-        <v>382</v>
       </c>
       <c r="J61" s="33" t="s">
         <v>105</v>
@@ -6612,10 +6615,14 @@
         <v>105</v>
       </c>
       <c r="N61" s="24" t="s">
-        <v>427</v>
-      </c>
-      <c r="O61" s="24"/>
-      <c r="P61" s="24"/>
+        <v>426</v>
+      </c>
+      <c r="O61" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P61" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q61" s="24"/>
       <c r="R61" s="25"/>
       <c r="S61" s="26"/>
@@ -6623,7 +6630,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="62" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A62" s="20">
         <v>103</v>
       </c>
@@ -6646,10 +6653,10 @@
         <v>45049.612187500003</v>
       </c>
       <c r="H62" s="38" t="s">
+        <v>382</v>
+      </c>
+      <c r="I62" s="36" t="s">
         <v>383</v>
-      </c>
-      <c r="I62" s="36" t="s">
-        <v>384</v>
       </c>
       <c r="J62" s="33" t="s">
         <v>105</v>
@@ -6662,10 +6669,14 @@
         <v>105</v>
       </c>
       <c r="N62" s="24" t="s">
-        <v>385</v>
-      </c>
-      <c r="O62" s="24"/>
-      <c r="P62" s="24"/>
+        <v>384</v>
+      </c>
+      <c r="O62" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P62" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q62" s="24"/>
       <c r="R62" s="25"/>
       <c r="S62" s="26"/>
@@ -6673,7 +6684,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="63" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A63" s="20">
         <v>104</v>
       </c>
@@ -6696,10 +6707,10 @@
         <v>45049.641134259262</v>
       </c>
       <c r="H63" s="38" t="s">
+        <v>385</v>
+      </c>
+      <c r="I63" s="36" t="s">
         <v>386</v>
-      </c>
-      <c r="I63" s="36" t="s">
-        <v>387</v>
       </c>
       <c r="J63" s="33" t="s">
         <v>105</v>
@@ -6712,10 +6723,14 @@
         <v>105</v>
       </c>
       <c r="N63" s="24" t="s">
-        <v>388</v>
-      </c>
-      <c r="O63" s="24"/>
-      <c r="P63" s="24"/>
+        <v>387</v>
+      </c>
+      <c r="O63" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P63" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q63" s="24"/>
       <c r="R63" s="25"/>
       <c r="S63" s="26"/>
@@ -6723,7 +6738,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="64" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A64" s="20">
         <v>105</v>
       </c>
@@ -6747,7 +6762,7 @@
         <v>302</v>
       </c>
       <c r="K64" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L64" s="24"/>
       <c r="M64" s="24"/>
@@ -6761,7 +6776,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="131" hidden="1" thickBot="1">
+    <row r="65" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A65" s="20">
         <v>106</v>
       </c>
@@ -6785,7 +6800,7 @@
         <v>302</v>
       </c>
       <c r="K65" s="39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L65" s="24"/>
       <c r="M65" s="24"/>
@@ -6799,7 +6814,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="66" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A66" s="20">
         <v>107</v>
       </c>
@@ -6823,7 +6838,7 @@
         <v>302</v>
       </c>
       <c r="K66" s="24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L66" s="24"/>
       <c r="M66" s="24"/>
@@ -6837,7 +6852,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="67" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A67" s="20">
         <v>108</v>
       </c>
@@ -6861,7 +6876,7 @@
         <v>302</v>
       </c>
       <c r="K67" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L67" s="24"/>
       <c r="M67" s="24"/>
@@ -6875,7 +6890,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="68" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A68" s="20">
         <v>109</v>
       </c>
@@ -6899,7 +6914,7 @@
         <v>302</v>
       </c>
       <c r="K68" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L68" s="24"/>
       <c r="M68" s="24"/>
@@ -6913,7 +6928,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="69" spans="1:20" ht="105.75" hidden="1" thickBot="1">
       <c r="A69" s="20">
         <v>110</v>
       </c>
@@ -6951,7 +6966,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="70" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A70" s="20">
         <v>111</v>
       </c>
@@ -6989,7 +7004,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="71" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A71" s="20">
         <v>112</v>
       </c>
@@ -7013,7 +7028,7 @@
         <v>302</v>
       </c>
       <c r="K71" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L71" s="24"/>
       <c r="M71" s="24"/>
@@ -7027,7 +7042,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="72" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A72" s="20">
         <v>113</v>
       </c>
@@ -7051,7 +7066,7 @@
         <v>302</v>
       </c>
       <c r="K72" s="24" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L72" s="24"/>
       <c r="M72" s="24"/>
@@ -7065,7 +7080,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="149.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="73" spans="1:20" ht="149.44999999999999" hidden="1" customHeight="1" thickBot="1">
       <c r="A73" s="20">
         <v>114</v>
       </c>
@@ -7088,10 +7103,10 @@
         <v>45050.579467592594</v>
       </c>
       <c r="H73" s="38" t="s">
+        <v>391</v>
+      </c>
+      <c r="I73" s="36" t="s">
         <v>392</v>
-      </c>
-      <c r="I73" s="36" t="s">
-        <v>393</v>
       </c>
       <c r="J73" s="33" t="s">
         <v>105</v>
@@ -7104,10 +7119,14 @@
         <v>105</v>
       </c>
       <c r="N73" s="24" t="s">
-        <v>394</v>
-      </c>
-      <c r="O73" s="24"/>
-      <c r="P73" s="24"/>
+        <v>393</v>
+      </c>
+      <c r="O73" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P73" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q73" s="24"/>
       <c r="R73" s="25"/>
       <c r="S73" s="26"/>
@@ -7139,7 +7158,7 @@
         <v>302</v>
       </c>
       <c r="K74" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L74" s="24"/>
       <c r="M74" s="24"/>
@@ -7153,7 +7172,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="145.5" hidden="1" thickBot="1">
+    <row r="75" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A75" s="20">
         <v>116</v>
       </c>
@@ -7176,10 +7195,10 @@
         <v>45050.596516203703</v>
       </c>
       <c r="H75" s="38" t="s">
+        <v>394</v>
+      </c>
+      <c r="I75" s="36" t="s">
         <v>395</v>
-      </c>
-      <c r="I75" s="36" t="s">
-        <v>396</v>
       </c>
       <c r="J75" s="33" t="s">
         <v>105</v>
@@ -7192,10 +7211,14 @@
         <v>105</v>
       </c>
       <c r="N75" s="24" t="s">
-        <v>397</v>
-      </c>
-      <c r="O75" s="24"/>
-      <c r="P75" s="24"/>
+        <v>396</v>
+      </c>
+      <c r="O75" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P75" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q75" s="24"/>
       <c r="R75" s="25"/>
       <c r="S75" s="26"/>
@@ -7203,7 +7226,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="76" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A76" s="20">
         <v>117</v>
       </c>
@@ -7226,10 +7249,10 @@
         <v>45050.62358796296</v>
       </c>
       <c r="H76" s="38" t="s">
+        <v>397</v>
+      </c>
+      <c r="I76" s="36" t="s">
         <v>398</v>
-      </c>
-      <c r="I76" s="36" t="s">
-        <v>399</v>
       </c>
       <c r="J76" s="33" t="s">
         <v>105</v>
@@ -7242,10 +7265,14 @@
         <v>105</v>
       </c>
       <c r="N76" s="24" t="s">
-        <v>400</v>
-      </c>
-      <c r="O76" s="24"/>
-      <c r="P76" s="24"/>
+        <v>399</v>
+      </c>
+      <c r="O76" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P76" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q76" s="24"/>
       <c r="R76" s="25"/>
       <c r="S76" s="26"/>
@@ -7253,7 +7280,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="77" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A77" s="20">
         <v>118</v>
       </c>
@@ -7276,10 +7303,10 @@
         <v>45050.632141203707</v>
       </c>
       <c r="H77" s="38" t="s">
+        <v>400</v>
+      </c>
+      <c r="I77" s="36" t="s">
         <v>401</v>
-      </c>
-      <c r="I77" s="36" t="s">
-        <v>402</v>
       </c>
       <c r="J77" s="33" t="s">
         <v>105</v>
@@ -7292,10 +7319,14 @@
         <v>105</v>
       </c>
       <c r="N77" s="24" t="s">
-        <v>403</v>
-      </c>
-      <c r="O77" s="24"/>
-      <c r="P77" s="24"/>
+        <v>402</v>
+      </c>
+      <c r="O77" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P77" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q77" s="24"/>
       <c r="R77" s="25"/>
       <c r="S77" s="26"/>
@@ -7303,7 +7334,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="78" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A78" s="20">
         <v>119</v>
       </c>
@@ -7327,7 +7358,7 @@
         <v>302</v>
       </c>
       <c r="K78" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L78" s="24"/>
       <c r="M78" s="24"/>
@@ -7341,7 +7372,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="79" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A79" s="20">
         <v>120</v>
       </c>
@@ -7365,7 +7396,7 @@
         <v>302</v>
       </c>
       <c r="K79" s="24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L79" s="24"/>
       <c r="M79" s="24"/>
@@ -7379,7 +7410,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="80" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A80" s="20">
         <v>121</v>
       </c>
@@ -7403,7 +7434,7 @@
         <v>302</v>
       </c>
       <c r="K80" s="24" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L80" s="24"/>
       <c r="M80" s="24"/>
@@ -7417,7 +7448,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="81" spans="1:20" ht="105.75" thickBot="1">
       <c r="A81" s="20">
         <v>122</v>
       </c>
@@ -7441,7 +7472,7 @@
         <v>302</v>
       </c>
       <c r="K81" s="24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L81" s="24"/>
       <c r="M81" s="24"/>
@@ -7455,7 +7486,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="82" spans="1:20" ht="105.75" thickBot="1">
       <c r="A82" s="20">
         <v>123</v>
       </c>
@@ -7479,7 +7510,7 @@
         <v>302</v>
       </c>
       <c r="K82" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L82" s="24"/>
       <c r="M82" s="24"/>
@@ -7493,7 +7524,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="83" spans="1:20" ht="105.75" thickBot="1">
       <c r="A83" s="20">
         <v>124</v>
       </c>
@@ -7517,7 +7548,7 @@
         <v>302</v>
       </c>
       <c r="K83" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L83" s="24"/>
       <c r="M83" s="24"/>
@@ -7531,7 +7562,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="84" spans="1:20" ht="120.75" thickBot="1">
       <c r="A84" s="20">
         <v>125</v>
       </c>
@@ -7569,7 +7600,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="85" spans="1:20" ht="105.75" thickBot="1">
       <c r="A85" s="20">
         <v>126</v>
       </c>
@@ -7607,7 +7638,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="86" spans="1:20" ht="105.75" thickBot="1">
       <c r="A86" s="20">
         <v>127</v>
       </c>
@@ -7631,7 +7662,7 @@
         <v>302</v>
       </c>
       <c r="K86" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L86" s="24"/>
       <c r="M86" s="24"/>
@@ -7645,7 +7676,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="87" spans="1:20" ht="150.75" thickBot="1">
       <c r="A87" s="20">
         <v>128</v>
       </c>
@@ -7668,10 +7699,10 @@
         <v>45051.431817129633</v>
       </c>
       <c r="H87" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="I87" s="36" t="s">
         <v>407</v>
-      </c>
-      <c r="I87" s="36" t="s">
-        <v>408</v>
       </c>
       <c r="J87" s="33" t="s">
         <v>105</v>
@@ -7684,10 +7715,14 @@
         <v>105</v>
       </c>
       <c r="N87" s="24" t="s">
-        <v>409</v>
-      </c>
-      <c r="O87" s="24"/>
-      <c r="P87" s="24"/>
+        <v>408</v>
+      </c>
+      <c r="O87" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P87" s="24" t="s">
+        <v>460</v>
+      </c>
       <c r="Q87" s="24"/>
       <c r="R87" s="25"/>
       <c r="S87" s="26"/>
@@ -7695,7 +7730,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="88" spans="1:20" ht="150.75" thickBot="1">
       <c r="A88" s="20">
         <v>129</v>
       </c>
@@ -7718,10 +7753,10 @@
         <v>45051.469490740739</v>
       </c>
       <c r="H88" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="I88" s="36" t="s">
         <v>410</v>
-      </c>
-      <c r="I88" s="36" t="s">
-        <v>411</v>
       </c>
       <c r="J88" s="33" t="s">
         <v>105</v>
@@ -7734,10 +7769,14 @@
         <v>105</v>
       </c>
       <c r="N88" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="O88" s="24"/>
-      <c r="P88" s="24"/>
+        <v>411</v>
+      </c>
+      <c r="O88" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P88" s="24" t="s">
+        <v>460</v>
+      </c>
       <c r="Q88" s="24"/>
       <c r="R88" s="25"/>
       <c r="S88" s="26"/>
@@ -7745,7 +7784,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="89" spans="1:20" ht="105.75" thickBot="1">
       <c r="A89" s="20">
         <v>130</v>
       </c>
@@ -7769,7 +7808,7 @@
         <v>302</v>
       </c>
       <c r="K89" s="24" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L89" s="24"/>
       <c r="M89" s="24"/>
@@ -7783,7 +7822,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="90" spans="1:20" ht="105.75" thickBot="1">
       <c r="A90" s="20">
         <v>131</v>
       </c>
@@ -7807,7 +7846,7 @@
         <v>302</v>
       </c>
       <c r="K90" s="24" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L90" s="24"/>
       <c r="M90" s="24"/>
@@ -7821,7 +7860,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="91" spans="1:20" ht="165.75" thickBot="1">
       <c r="A91" s="20">
         <v>132</v>
       </c>
@@ -7844,10 +7883,10 @@
         <v>45051.497754629629</v>
       </c>
       <c r="H91" s="38" t="s">
+        <v>414</v>
+      </c>
+      <c r="I91" s="36" t="s">
         <v>415</v>
-      </c>
-      <c r="I91" s="36" t="s">
-        <v>416</v>
       </c>
       <c r="J91" s="33" t="s">
         <v>105</v>
@@ -7860,10 +7899,14 @@
         <v>105</v>
       </c>
       <c r="N91" s="24" t="s">
-        <v>417</v>
-      </c>
-      <c r="O91" s="24"/>
-      <c r="P91" s="24"/>
+        <v>416</v>
+      </c>
+      <c r="O91" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P91" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q91" s="24"/>
       <c r="R91" s="25"/>
       <c r="S91" s="26"/>
@@ -7871,7 +7914,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="92" spans="1:20" ht="165.75" thickBot="1">
       <c r="A92" s="20">
         <v>133</v>
       </c>
@@ -7894,10 +7937,10 @@
         <v>45051.516504629632</v>
       </c>
       <c r="H92" s="38" t="s">
+        <v>417</v>
+      </c>
+      <c r="I92" s="36" t="s">
         <v>418</v>
-      </c>
-      <c r="I92" s="36" t="s">
-        <v>419</v>
       </c>
       <c r="J92" s="33" t="s">
         <v>105</v>
@@ -7910,10 +7953,14 @@
         <v>105</v>
       </c>
       <c r="N92" s="24" t="s">
-        <v>420</v>
-      </c>
-      <c r="O92" s="24"/>
-      <c r="P92" s="24"/>
+        <v>419</v>
+      </c>
+      <c r="O92" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P92" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q92" s="24"/>
       <c r="R92" s="25"/>
       <c r="S92" s="26"/>
@@ -7921,7 +7968,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="93" spans="1:20" ht="105.75" thickBot="1">
       <c r="A93" s="20">
         <v>134</v>
       </c>
@@ -7945,7 +7992,7 @@
         <v>302</v>
       </c>
       <c r="K93" s="24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L93" s="24"/>
       <c r="M93" s="24"/>
@@ -7959,7 +8006,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="94" spans="1:20" ht="105.75" thickBot="1">
       <c r="A94" s="20">
         <v>135</v>
       </c>
@@ -7983,7 +8030,7 @@
         <v>302</v>
       </c>
       <c r="K94" s="24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L94" s="24"/>
       <c r="M94" s="24"/>
@@ -7997,7 +8044,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="95" spans="1:20" ht="105.75" thickBot="1">
       <c r="A95" s="20">
         <v>136</v>
       </c>
@@ -8021,7 +8068,7 @@
         <v>302</v>
       </c>
       <c r="K95" s="24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L95" s="24"/>
       <c r="M95" s="24"/>
@@ -8035,7 +8082,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="96" spans="1:20" ht="120.75" thickBot="1">
       <c r="A96" s="20">
         <v>137</v>
       </c>
@@ -8059,7 +8106,7 @@
         <v>302</v>
       </c>
       <c r="K96" s="24" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L96" s="24"/>
       <c r="M96" s="24"/>
@@ -8073,7 +8120,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="97" spans="1:20" ht="165.75" thickBot="1">
       <c r="A97" s="20">
         <v>138</v>
       </c>
@@ -8096,10 +8143,10 @@
         <v>45051.534421296295</v>
       </c>
       <c r="H97" s="38" t="s">
+        <v>423</v>
+      </c>
+      <c r="I97" s="36" t="s">
         <v>424</v>
-      </c>
-      <c r="I97" s="36" t="s">
-        <v>425</v>
       </c>
       <c r="J97" s="33" t="s">
         <v>105</v>
@@ -8112,10 +8159,14 @@
         <v>105</v>
       </c>
       <c r="N97" s="24" t="s">
-        <v>426</v>
-      </c>
-      <c r="O97" s="24"/>
-      <c r="P97" s="24"/>
+        <v>425</v>
+      </c>
+      <c r="O97" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P97" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q97" s="24"/>
       <c r="R97" s="25"/>
       <c r="S97" s="26"/>
@@ -8123,7 +8174,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="98" spans="1:20" ht="105.75" thickBot="1">
       <c r="A98" s="20">
         <v>139</v>
       </c>
@@ -8147,7 +8198,7 @@
         <v>302</v>
       </c>
       <c r="K98" s="24" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L98" s="24"/>
       <c r="M98" s="24"/>
@@ -8161,7 +8212,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="99" spans="1:20" ht="165.75" thickBot="1">
       <c r="A99" s="20">
         <v>140</v>
       </c>
@@ -8184,10 +8235,10 @@
         <v>45051.599918981483</v>
       </c>
       <c r="H99" s="38" t="s">
+        <v>428</v>
+      </c>
+      <c r="I99" s="36" t="s">
         <v>429</v>
-      </c>
-      <c r="I99" s="36" t="s">
-        <v>430</v>
       </c>
       <c r="J99" s="33" t="s">
         <v>105</v>
@@ -8200,10 +8251,14 @@
         <v>105</v>
       </c>
       <c r="N99" s="24" t="s">
-        <v>431</v>
-      </c>
-      <c r="O99" s="24"/>
-      <c r="P99" s="24"/>
+        <v>430</v>
+      </c>
+      <c r="O99" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P99" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q99" s="24"/>
       <c r="R99" s="25"/>
       <c r="S99" s="26"/>
@@ -8211,7 +8266,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="100" spans="1:20" ht="120.75" thickBot="1">
       <c r="A100" s="20">
         <v>141</v>
       </c>
@@ -8235,7 +8290,7 @@
         <v>302</v>
       </c>
       <c r="K100" s="24" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L100" s="24"/>
       <c r="M100" s="24"/>
@@ -8249,7 +8304,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="101" spans="1:20" ht="165.75" thickBot="1">
       <c r="A101" s="20">
         <v>142</v>
       </c>
@@ -8272,10 +8327,10 @@
         <v>45051.615173611113</v>
       </c>
       <c r="H101" s="38" t="s">
+        <v>432</v>
+      </c>
+      <c r="I101" s="36" t="s">
         <v>433</v>
-      </c>
-      <c r="I101" s="36" t="s">
-        <v>434</v>
       </c>
       <c r="J101" s="33" t="s">
         <v>105</v>
@@ -8288,10 +8343,14 @@
         <v>105</v>
       </c>
       <c r="N101" s="24" t="s">
-        <v>435</v>
-      </c>
-      <c r="O101" s="24"/>
-      <c r="P101" s="24"/>
+        <v>434</v>
+      </c>
+      <c r="O101" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P101" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q101" s="24"/>
       <c r="R101" s="25"/>
       <c r="S101" s="26"/>
@@ -8299,7 +8358,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="102" spans="1:20" ht="165.75" thickBot="1">
       <c r="A102" s="20">
         <v>143</v>
       </c>
@@ -8322,10 +8381,10 @@
         <v>45051.632314814815</v>
       </c>
       <c r="H102" s="38" t="s">
+        <v>435</v>
+      </c>
+      <c r="I102" s="36" t="s">
         <v>436</v>
-      </c>
-      <c r="I102" s="36" t="s">
-        <v>437</v>
       </c>
       <c r="J102" s="33" t="s">
         <v>105</v>
@@ -8338,10 +8397,14 @@
         <v>105</v>
       </c>
       <c r="N102" s="24" t="s">
-        <v>438</v>
-      </c>
-      <c r="O102" s="24"/>
-      <c r="P102" s="24"/>
+        <v>437</v>
+      </c>
+      <c r="O102" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P102" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q102" s="24"/>
       <c r="R102" s="25"/>
       <c r="S102" s="26"/>
@@ -8349,7 +8412,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="102" hidden="1" thickBot="1">
+    <row r="103" spans="1:20" ht="165.75" thickBot="1">
       <c r="A103" s="20">
         <v>144</v>
       </c>
@@ -8372,10 +8435,10 @@
         <v>45051.642523148148</v>
       </c>
       <c r="H103" s="38" t="s">
+        <v>438</v>
+      </c>
+      <c r="I103" s="36" t="s">
         <v>439</v>
-      </c>
-      <c r="I103" s="36" t="s">
-        <v>440</v>
       </c>
       <c r="J103" s="33" t="s">
         <v>105</v>
@@ -8388,10 +8451,14 @@
         <v>105</v>
       </c>
       <c r="N103" s="24" t="s">
-        <v>441</v>
-      </c>
-      <c r="O103" s="24"/>
-      <c r="P103" s="24"/>
+        <v>440</v>
+      </c>
+      <c r="O103" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P103" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q103" s="24"/>
       <c r="R103" s="25"/>
       <c r="S103" s="26"/>
@@ -8399,7 +8466,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="104" spans="1:20" ht="120.75" thickBot="1">
       <c r="A104" s="20">
         <v>145</v>
       </c>
@@ -8423,7 +8490,7 @@
         <v>302</v>
       </c>
       <c r="K104" s="24" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L104" s="24"/>
       <c r="M104" s="24"/>
@@ -8437,7 +8504,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="116.5" hidden="1" thickBot="1">
+    <row r="105" spans="1:20" ht="120">
       <c r="A105" s="20">
         <v>146</v>
       </c>
@@ -8461,7 +8528,7 @@
         <v>302</v>
       </c>
       <c r="K105" s="24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L105" s="24"/>
       <c r="M105" s="24"/>
@@ -8475,7 +8542,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="160" thickBot="1">
+    <row r="106" spans="1:20" ht="165" hidden="1">
       <c r="A106" s="20">
         <v>147</v>
       </c>
@@ -8498,10 +8565,10 @@
         <v>45042.607048611113</v>
       </c>
       <c r="H106" s="38" t="s">
+        <v>356</v>
+      </c>
+      <c r="I106" s="36" t="s">
         <v>357</v>
-      </c>
-      <c r="I106" s="36" t="s">
-        <v>358</v>
       </c>
       <c r="J106" s="33" t="s">
         <v>105</v>
@@ -8519,7 +8586,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="160" thickBot="1">
+    <row r="107" spans="1:20" ht="165" hidden="1">
       <c r="A107" s="20">
         <v>148</v>
       </c>
@@ -8542,16 +8609,16 @@
         <v>45042.776261574072</v>
       </c>
       <c r="H107" s="38" t="s">
+        <v>358</v>
+      </c>
+      <c r="I107" s="36" t="s">
         <v>359</v>
-      </c>
-      <c r="I107" s="36" t="s">
-        <v>360</v>
       </c>
       <c r="J107" s="33" t="s">
         <v>302</v>
       </c>
       <c r="K107" s="24" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L107" s="24"/>
       <c r="M107" s="24"/>
@@ -8565,7 +8632,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="160" thickBot="1">
+    <row r="108" spans="1:20" ht="165" hidden="1">
       <c r="A108" s="20">
         <v>149</v>
       </c>
@@ -8588,16 +8655,16 @@
         <v>45043.598506944443</v>
       </c>
       <c r="H108" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="I108" s="36" t="s">
         <v>362</v>
-      </c>
-      <c r="I108" s="36" t="s">
-        <v>363</v>
       </c>
       <c r="J108" s="33" t="s">
         <v>302</v>
       </c>
       <c r="K108" s="24" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L108" s="24"/>
       <c r="M108" s="24"/>
@@ -8611,7 +8678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="160" thickBot="1">
+    <row r="109" spans="1:20" ht="165" hidden="1">
       <c r="A109" s="20">
         <v>150</v>
       </c>
@@ -8634,10 +8701,10 @@
         <v>45043.66443287037</v>
       </c>
       <c r="H109" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="I109" s="36" t="s">
         <v>365</v>
-      </c>
-      <c r="I109" s="36" t="s">
-        <v>366</v>
       </c>
       <c r="J109" s="33" t="s">
         <v>105</v>
@@ -8655,7 +8722,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="102" thickBot="1">
+    <row r="110" spans="1:20" ht="120" hidden="1">
       <c r="A110" s="20">
         <v>151</v>
       </c>
@@ -8679,7 +8746,7 @@
         <v>302</v>
       </c>
       <c r="K110" s="24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L110" s="24"/>
       <c r="M110" s="24"/>
@@ -8693,7 +8760,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="116.5" thickBot="1">
+    <row r="111" spans="1:20" ht="135" hidden="1">
       <c r="A111" s="20">
         <v>152</v>
       </c>
@@ -8717,7 +8784,7 @@
         <v>302</v>
       </c>
       <c r="K111" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L111" s="24"/>
       <c r="M111" s="24"/>
@@ -8731,7 +8798,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="116.5" thickBot="1">
+    <row r="112" spans="1:20" ht="135" hidden="1">
       <c r="A112" s="20">
         <v>153</v>
       </c>
@@ -8755,7 +8822,7 @@
         <v>302</v>
       </c>
       <c r="K112" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L112" s="24"/>
       <c r="M112" s="24"/>
@@ -8769,7 +8836,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="116.5" thickBot="1">
+    <row r="113" spans="1:20" ht="135" hidden="1">
       <c r="A113" s="20">
         <v>154</v>
       </c>
@@ -8807,7 +8874,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="116.5" thickBot="1">
+    <row r="114" spans="1:20" ht="135" hidden="1">
       <c r="A114" s="20">
         <v>155</v>
       </c>
@@ -8845,7 +8912,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="116.5" thickBot="1">
+    <row r="115" spans="1:20" ht="135" hidden="1">
       <c r="A115" s="20">
         <v>156</v>
       </c>
@@ -8869,7 +8936,7 @@
         <v>302</v>
       </c>
       <c r="K115" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L115" s="24"/>
       <c r="M115" s="24"/>
@@ -8883,7 +8950,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="116.5" thickBot="1">
+    <row r="116" spans="1:20" ht="135" hidden="1">
       <c r="A116" s="20">
         <v>157</v>
       </c>
@@ -8907,7 +8974,7 @@
         <v>302</v>
       </c>
       <c r="K116" s="24" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L116" s="24"/>
       <c r="M116" s="24"/>
@@ -8921,7 +8988,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="116.5" thickBot="1">
+    <row r="117" spans="1:20" ht="165" hidden="1">
       <c r="A117" s="20">
         <v>158</v>
       </c>
@@ -8944,10 +9011,10 @@
         <v>45051.739178240743</v>
       </c>
       <c r="H117" s="40" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I117" s="36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J117" s="33" t="s">
         <v>105</v>
@@ -8960,10 +9027,14 @@
         <v>105</v>
       </c>
       <c r="N117" s="24" t="s">
-        <v>446</v>
-      </c>
-      <c r="O117" s="24"/>
-      <c r="P117" s="24"/>
+        <v>445</v>
+      </c>
+      <c r="O117" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P117" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q117" s="24"/>
       <c r="R117" s="25"/>
       <c r="S117" s="26"/>
@@ -8971,7 +9042,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="102" thickBot="1">
+    <row r="118" spans="1:20" ht="120" hidden="1">
       <c r="A118" s="20">
         <v>159</v>
       </c>
@@ -8995,7 +9066,7 @@
         <v>302</v>
       </c>
       <c r="K118" s="24" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L118" s="24"/>
       <c r="M118" s="24"/>
@@ -9009,7 +9080,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="102" thickBot="1">
+    <row r="119" spans="1:20" ht="165" hidden="1">
       <c r="A119" s="20">
         <v>160</v>
       </c>
@@ -9032,10 +9103,10 @@
         <v>45051.75072916667</v>
       </c>
       <c r="H119" s="38" t="s">
+        <v>448</v>
+      </c>
+      <c r="I119" s="36" t="s">
         <v>449</v>
-      </c>
-      <c r="I119" s="36" t="s">
-        <v>450</v>
       </c>
       <c r="J119" s="33" t="s">
         <v>105</v>
@@ -9048,10 +9119,14 @@
         <v>105</v>
       </c>
       <c r="N119" s="24" t="s">
-        <v>451</v>
-      </c>
-      <c r="O119" s="24"/>
-      <c r="P119" s="24"/>
+        <v>450</v>
+      </c>
+      <c r="O119" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P119" s="24" t="s">
+        <v>462</v>
+      </c>
       <c r="Q119" s="24"/>
       <c r="R119" s="25"/>
       <c r="S119" s="26"/>
@@ -9059,7 +9134,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="116.5" thickBot="1">
+    <row r="120" spans="1:20" ht="135" hidden="1">
       <c r="A120" s="20">
         <v>161</v>
       </c>
@@ -9083,7 +9158,7 @@
         <v>302</v>
       </c>
       <c r="K120" s="24" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L120" s="24"/>
       <c r="M120" s="24"/>
@@ -9097,7 +9172,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="116.5" thickBot="1">
+    <row r="121" spans="1:20" ht="135" hidden="1">
       <c r="A121" s="20">
         <v>162</v>
       </c>
@@ -9121,7 +9196,7 @@
         <v>302</v>
       </c>
       <c r="K121" s="24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L121" s="24"/>
       <c r="M121" s="24"/>
@@ -9135,7 +9210,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="116.5" thickBot="1">
+    <row r="122" spans="1:20" ht="135" hidden="1">
       <c r="A122" s="20">
         <v>163</v>
       </c>
@@ -9159,7 +9234,7 @@
         <v>302</v>
       </c>
       <c r="K122" s="24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L122" s="24"/>
       <c r="M122" s="24"/>
@@ -9173,7 +9248,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="116.5" thickBot="1">
+    <row r="123" spans="1:20" ht="135" hidden="1">
       <c r="A123" s="20">
         <v>164</v>
       </c>
@@ -9197,7 +9272,7 @@
         <v>302</v>
       </c>
       <c r="K123" s="24" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L123" s="24"/>
       <c r="M123" s="24"/>
@@ -9211,7 +9286,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="116.5" thickBot="1">
+    <row r="124" spans="1:20" ht="135" hidden="1">
       <c r="A124" s="20">
         <v>165</v>
       </c>
@@ -9235,7 +9310,7 @@
         <v>302</v>
       </c>
       <c r="K124" s="24" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="L124" s="24"/>
       <c r="M124" s="24"/>
@@ -9249,7 +9324,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="116.5" thickBot="1">
+    <row r="125" spans="1:20" ht="135" hidden="1">
       <c r="A125" s="20">
         <v>166</v>
       </c>
@@ -9273,7 +9348,7 @@
         <v>302</v>
       </c>
       <c r="K125" s="24" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="L125" s="24"/>
       <c r="M125" s="24"/>
@@ -9287,7 +9362,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="116.5" thickBot="1">
+    <row r="126" spans="1:20" ht="135" hidden="1">
       <c r="A126" s="20">
         <v>167</v>
       </c>
@@ -9311,7 +9386,7 @@
         <v>302</v>
       </c>
       <c r="K126" s="24" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="L126" s="24"/>
       <c r="M126" s="24"/>
@@ -9325,7 +9400,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="116.5" thickBot="1">
+    <row r="127" spans="1:20" ht="150" hidden="1">
       <c r="A127" s="20">
         <v>168</v>
       </c>
@@ -9348,10 +9423,10 @@
         <v>45051.783020833333</v>
       </c>
       <c r="H127" s="38" t="s">
+        <v>456</v>
+      </c>
+      <c r="I127" s="36" t="s">
         <v>457</v>
-      </c>
-      <c r="I127" s="36" t="s">
-        <v>458</v>
       </c>
       <c r="J127" s="33" t="s">
         <v>105</v>
@@ -9364,10 +9439,14 @@
         <v>105</v>
       </c>
       <c r="N127" s="24" t="s">
-        <v>459</v>
-      </c>
-      <c r="O127" s="24"/>
-      <c r="P127" s="24"/>
+        <v>458</v>
+      </c>
+      <c r="O127" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P127" s="24" t="s">
+        <v>460</v>
+      </c>
       <c r="Q127" s="24"/>
       <c r="R127" s="25"/>
       <c r="S127" s="26"/>
@@ -9375,7 +9454,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="116">
+    <row r="128" spans="1:20" ht="135" hidden="1">
       <c r="A128" s="20">
         <v>169</v>
       </c>
@@ -9399,7 +9478,7 @@
         <v>302</v>
       </c>
       <c r="K128" s="24" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L128" s="24"/>
       <c r="M128" s="24"/>
@@ -19013,7 +19092,7 @@
   <autoFilter ref="A9:T128">
     <filterColumn colId="2">
       <filters>
-        <filter val="RSA"/>
+        <filter val="VPS"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -19036,7 +19115,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J51:J128 L33:M128 O33:O128 O28:O31 L28:M31 J28:J31 O10:O26 L10:M26 J33:J40 J43 J11:J25</xm:sqref>
+          <xm:sqref>J51:J128 L33:M128 O33:O128 O28:O31 L28:M31 J28:J31 O10:O26 L10:M26 J11:J25 J43 J33:J41</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
@@ -19046,9 +19125,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[1]Sheet1!#REF!</xm:f>
+            <xm:f>'[accreditamento-checklist_V4.2_personalizzato.xlsx]Sheet1'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>J10 J41:J42 J44:J50 J26</xm:sqref>
+          <xm:sqref>J10 J26 J44:J50 J42</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -19065,15 +19144,15 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="23.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="102" customWidth="1"/>
-    <col min="5" max="6" width="8.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" customWidth="1"/>
-    <col min="8" max="26" width="8.81640625" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1">
@@ -19132,7 +19211,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.5">
+    <row r="5" spans="1:4">
       <c r="A5" s="11" t="s">
         <v>49</v>
       </c>
@@ -19146,7 +19225,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.5">
+    <row r="6" spans="1:4">
       <c r="A6" s="11" t="s">
         <v>50</v>
       </c>
@@ -20120,11 +20199,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1"/>
-    <col min="3" max="26" width="8.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Cambiato file report-checklist.xlsx - V4
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ADSFINMATIC/Data_Processing_SPA/SmartHealth/4.5.048/report-checklist.xlsx
+++ b/GATEWAY/A1#111ADSFINMATIC/Data_Processing_SPA/SmartHealth/4.5.048/report-checklist.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="454">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1658,12 +1658,6 @@
     <t>Data Processing SPA</t>
   </si>
   <si>
-    <t>a8c288c6628ba360</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4e5fd81aa073d064611f84c74a025665352b63c1ec879596b894d815f38adc11.9c1f394027^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Comune di Residenza è un dato obbligatorio</t>
   </si>
   <si>
@@ -1688,36 +1682,6 @@
     <t>I ns modelli di LDO possono prevedere nella sezione "Inquadramento Clinico Iniziale",  eventuali sottosezioni (Anamnesi, Esame Obiettivo, Terapia farmacologica in ingresso) in forma testuale (no Entry)</t>
   </si>
   <si>
-    <t>105e19941def735d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.231362e113b96182b9130cc22ff27b166d1af3a5f7fe44efaee20c776e0fad40.fb39eaa807^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>3aa46cc096d7abcc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.d7469a29426e3dcc9a3a6aed4be06ddb8107f37a84dec799826754ba6ac9afdb.e7f311292c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>3531592f127b7756</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.e723f410e2273623c6167a8d8ffeb1d4fe624c1562d7979cb2e5726c3a1380f3.d2f94834f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6bedd0bfb9af1247</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c99f3d96fbc81adfe5a192f1fbc4192b4b9c9714351e4c79f4c3778eec4fbd43.af36022983^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>cf6760283c52492e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c008dd2336fdd25e4bfb6f3233c18aedabb418511676782448be94bd077c11c3.e6fcd5f474^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>La composizione del CDA in Applicativo prevede OBBLIGATORIAMENTE la valorizzazione del confidentialityCode con i soli valori N (Normal) per documenti non oscurati e V (Very restricted) per documenti oscurati</t>
   </si>
   <si>
@@ -1742,98 +1706,14 @@
     <t>Il modello RSA realizzato, prevede sì la sezione Storia Clinica, ma non la suddivide in sotto-sezioni, per cui non è prevista anamnesi patologica , né tantomeno data di insorgenza del problema in modo strutturato</t>
   </si>
   <si>
-    <t>2a40b5356277e593</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.868cc79572365720062c7b62a4820c42311b825b3cb5a1f8c66c1db30ba3180d.e85ea2280a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>fef45909fbc4c6f6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.a0e20f0075ff50b888c1b21748a10f8c3ec87eb4a2f807f6987194ae8125353c.e7a4adcc15^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>77356588f1cc88dd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.aca2b722df37c0bffd7fff568a2b6ad264b7ddf739510e497b22bbc3f6853c7c.d516a08e72^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2ce8a5b746da3f1a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.aca2b722df37c0bffd7fff568a2b6ad264b7ddf739510e497b22bbc3f6853c7c.24744281da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>65d90822e3d8f8e9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.aca2b722df37c0bffd7fff568a2b6ad264b7ddf739510e497b22bbc3f6853c7c.eab118f1c9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2bb34e9e9737321c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.aca2b722df37c0bffd7fff568a2b6ad264b7ddf739510e497b22bbc3f6853c7c.3e78ab93ad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6722f014442f0dff</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.98a70d7736dd385faeb51a11240742971ee2abb56276785314ed389bc0c0e617.c263832b3a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>1050f14909106b5c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ed9d6500ad63caaf49fe840fe14df681ae8e22f23b3ef3b10a4a41e8b9c4706a.ea4102156a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Smart*Health gestisce i dati delle sottosezioni di "Inquadramento clinico iniziale" in maniera testuale, non è in grado di fornire la parte di CDA relativa alle entry di Anamnesi e Allergie. Discorso analogo per sezione " Terapia farmacologica alla dimissione ", nel CDA è presente solo la parte testuale ed è assente la parte di entry.</t>
-  </si>
-  <si>
-    <t>cc283102f353e966</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.83f59a8bee5ceb2fe95d6f5bfeaa1abd5573d1a6f3285933ce0264f99bf95c41.cd8dbd76b8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>1bb257162c10294b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.6c773a99318d58e17d351d632b9920f15b87cf43f996a4845b6f506b7b8fa6ce.f10a44cd1a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>7a36e047e593eb5b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.be49805d357b34c323595fd8d418717ecaa87baf36dabe7ce3de212d94894529.ffe8a13c35^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>23c66eb177d80df2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.280ea8107d61febb4dca5f8daafdf578edff7b4433036b15c5c13a39426b829b.1b686386b9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Smart*Health gestisce i dati delle sottosezioni di "Storia Clinica" in maniera testuale, non è in grado di fornire la parte di CDA relativa alle entry di Allergie (Criticità e Stato) e Terapia Farmacologica in atto. Discorso analogo per sezione "Diagnosi" e "Accertamenti e Controlli consigliati", nel CDA è presente solo la parte testuale ed è assente la parte di entry.
 </t>
   </si>
   <si>
-    <t>5972bc6923ce4134</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.16f9589c45fd874803c84dddbe93eca5030e63140300273ba2fb56d6b60efe16.6020bcc922^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Smart*Health gestisce i dati delle sezioni "Diagnosi", "Accertamenti e Controlli consigliati" e "Terapia Farmacologica Consigliata" in maniera testuale, non è in grado di fornire la parte di CDA relativa alle entry.</t>
-  </si>
-  <si>
-    <t>b638ad450cd03893</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.770cddcc7527c7668aa8a7ba8ac1a70c935db14f218a7b66db5e1cb92eeb7a38.6ce4b344ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Nel modello LDO la parte testuale per la compilazione delle "Condizioni del paziente alla dimissione" è un contenuto obbligatorio. Lla presenza della diagnosi principale di dimissione in ICD9CM è invece configurabile con specifico controllo.</t>
@@ -2128,14 +2008,108 @@
   <si>
     <t xml:space="preserve">In questa fase, in cui non è necessaria la firma digitale dei documenti, quelli per cui l'invio fallisce vengono riportati in stato NON validato per essere disponibili a nuova validazione ed invio : viene data evidenza dei documenti in questo stato.
 </t>
+  </si>
+  <si>
+    <t>e64549fd5dc5e80c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.a253d789cc322352b5528d6dd84988d50b4369090039021bee6ddd7b5dbd8ef5.0e434e3df6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>94e946b2980b8764</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.fa23160dfa802cb094e5e55dae58b2e7a9e5758d266cf8c0ab3e302cd22bcbe1.e69c7afe13^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3b42022d3cf31a5f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c16a01cc30f15016b7399052e496a5e15537a393cf8c108ad81c0744ae4577a5.4ee0b93942^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>fec989ec08e07858</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.a2e08c438204911afcfeca1ac45bf34b8bf0300c514e9d99ebb8bc8a9a426832.abf5c96f06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>547fecf6c47e71ad</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.13e0f5a9426b64ec30630c4341a89a4ea51efe0ff9c9f6f40ebbee6435c7e4e0.446313bf75^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>6cb5b08f9ae6bebe</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.aca2b722df37c0bffd7fff568a2b6ad264b7ddf739510e497b22bbc3f6853c7c.43b720e94c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>87ff86a57999eae8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.aca2b722df37c0bffd7fff568a2b6ad264b7ddf739510e497b22bbc3f6853c7c.b02ed856e0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>fb1d54ac12017c7f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.aca2b722df37c0bffd7fff568a2b6ad264b7ddf739510e497b22bbc3f6853c7c.37c7e6100b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>0ca25115bb87502d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.aca2b722df37c0bffd7fff568a2b6ad264b7ddf739510e497b22bbc3f6853c7c.28d6e569cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>89fafa928fcede6f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c64af3e86a2cd7a1199ae83064fa323cccd1b72514e99a70754aa5a2be74df01.04656919c9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ccfae393fc311d42</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.ea9dc58a1901dd2fbe68e5fd4a6e3473787143777bad7bcfde29e13901642b85.1b9bced029^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>672b51ae559fefe9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.8ef80b5199975da79766588dd72059872aeb4b2d09870f421277a8496265dba2.78d4add3f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ed6bf58de76e5f7f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.9c470625de737f007b9370616183cc52e9705f65c72c8a47a9a2e9d46244ff06.db8d3487e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>41c58140ef7ddde9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.76974e3457ba2b3ebb1e0b04814a76f4f99b34c874597b819799c9b1ec66f3a1.9d95849f2e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Smart*Health gestisce i dati delle sottosezioni di "Inquadramento clinico iniziale" in maniera testuale, non è in grado di fornire la parte di CDA relativa alle entry di Anamnesi e Allergie. Discorso analogo per sezioni " Parametri Vitali " e  " Terapia farmacologica alla dimissione ", nel CDA è presente solo la parte testuale ed è assente la parte di entry.</t>
+  </si>
+  <si>
+    <t>a8640d6f58cc9a3a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.cb04cd71d909e7cbec90a3aa7aa50e41723f3c412f1275865548351528c71d78.219435102f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -2463,7 +2437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2579,6 +2553,12 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2915,10 +2895,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="130.140625" customWidth="1"/>
-    <col min="2" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="130.1796875" customWidth="1"/>
+    <col min="2" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2926,27 +2906,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="90">
+    <row r="2" spans="1:1" ht="87">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="30">
+    <row r="3" spans="1:1" ht="29">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="195">
+    <row r="4" spans="1:1" ht="174">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="30">
+    <row r="5" spans="1:1" ht="29">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30">
+    <row r="6" spans="1:1" ht="29">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2964,7 +2944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="45">
+    <row r="10" spans="1:1" ht="29">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2992,11 +2972,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="194.140625" customWidth="1"/>
-    <col min="3" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
+    <col min="2" max="2" width="194.1796875" customWidth="1"/>
+    <col min="3" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -3068,7 +3048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="45">
+    <row r="11" spans="1:2" ht="43.5">
       <c r="A11" s="10">
         <v>8</v>
       </c>
@@ -4088,28 +4068,28 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="L96" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="G108" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P97" sqref="P97"/>
+      <selection pane="bottomRight" activeCell="L107" sqref="L107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" customWidth="1"/>
-    <col min="5" max="5" width="104.85546875" customWidth="1"/>
-    <col min="6" max="9" width="33.140625" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="15" width="36.42578125" customWidth="1"/>
-    <col min="16" max="16" width="27.140625" customWidth="1"/>
-    <col min="17" max="17" width="33.140625" customWidth="1"/>
-    <col min="18" max="18" width="36.42578125" customWidth="1"/>
-    <col min="19" max="20" width="31.85546875" customWidth="1"/>
-    <col min="21" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="46.81640625" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" customWidth="1"/>
+    <col min="4" max="4" width="63.81640625" customWidth="1"/>
+    <col min="5" max="5" width="104.81640625" customWidth="1"/>
+    <col min="6" max="9" width="33.1796875" customWidth="1"/>
+    <col min="10" max="10" width="27.1796875" customWidth="1"/>
+    <col min="11" max="15" width="36.453125" customWidth="1"/>
+    <col min="16" max="16" width="27.1796875" customWidth="1"/>
+    <col min="17" max="17" width="33.1796875" customWidth="1"/>
+    <col min="18" max="18" width="36.453125" customWidth="1"/>
+    <col min="19" max="20" width="31.81640625" customWidth="1"/>
+    <col min="21" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" customHeight="1">
@@ -4131,14 +4111,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="47" t="s">
         <v>306</v>
       </c>
-      <c r="D2" s="44"/>
+      <c r="D2" s="46"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4156,14 +4136,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="52" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="54" t="s">
         <v>303</v>
       </c>
-      <c r="D3" s="44"/>
+      <c r="D3" s="46"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4181,12 +4161,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="52" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="54" t="s">
         <v>304</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4205,12 +4185,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="50"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="52" t="s">
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="54" t="s">
         <v>305</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="46"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4228,8 +4208,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4346,7 +4326,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="10" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A10" s="20">
         <v>6</v>
       </c>
@@ -4363,16 +4343,16 @@
         <v>53</v>
       </c>
       <c r="F10" s="31">
-        <v>44985</v>
+        <v>45063</v>
       </c>
       <c r="G10" s="32">
-        <v>44985.459467592591</v>
+        <v>45063.694826388892</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>307</v>
+        <v>423</v>
       </c>
       <c r="I10" s="36" t="s">
-        <v>308</v>
+        <v>424</v>
       </c>
       <c r="J10" s="33" t="s">
         <v>105</v>
@@ -4390,7 +4370,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="11" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A11" s="20">
         <v>7</v>
       </c>
@@ -4407,16 +4387,16 @@
         <v>55</v>
       </c>
       <c r="F11" s="23">
-        <v>44985</v>
+        <v>45068</v>
       </c>
       <c r="G11" s="35">
-        <v>44985.513518518521</v>
-      </c>
-      <c r="H11" s="37" t="s">
-        <v>317</v>
+        <v>45068.63548611111</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>425</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>318</v>
+        <v>426</v>
       </c>
       <c r="J11" s="33" t="s">
         <v>105</v>
@@ -4434,7 +4414,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="12" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A12" s="20">
         <v>8</v>
       </c>
@@ -4451,16 +4431,16 @@
         <v>57</v>
       </c>
       <c r="F12" s="23">
-        <v>44986</v>
+        <v>45078</v>
       </c>
       <c r="G12" s="35">
-        <v>44986.648530092592</v>
-      </c>
-      <c r="H12" s="37" t="s">
-        <v>319</v>
+        <v>45078.56486111111</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>443</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>320</v>
+        <v>444</v>
       </c>
       <c r="J12" s="33" t="s">
         <v>105</v>
@@ -4478,7 +4458,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="13" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A13" s="20">
         <v>9</v>
       </c>
@@ -4495,16 +4475,16 @@
         <v>59</v>
       </c>
       <c r="F13" s="23">
-        <v>45020</v>
+        <v>45078</v>
       </c>
       <c r="G13" s="35">
-        <v>45020.720949074072</v>
+        <v>45078.671469907407</v>
       </c>
       <c r="H13" s="37" t="s">
-        <v>321</v>
+        <v>445</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>322</v>
+        <v>446</v>
       </c>
       <c r="J13" s="33" t="s">
         <v>105</v>
@@ -4522,7 +4502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="135.75" hidden="1" thickBot="1">
+    <row r="14" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A14" s="20">
         <v>16</v>
       </c>
@@ -4539,16 +4519,16 @@
         <v>61</v>
       </c>
       <c r="F14" s="23">
-        <v>45033</v>
+        <v>45078</v>
       </c>
       <c r="G14" s="35">
-        <v>45033.477523148147</v>
-      </c>
-      <c r="H14" s="38" t="s">
-        <v>323</v>
+        <v>45078.467199074075</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>441</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>324</v>
+        <v>442</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>105</v>
@@ -4566,7 +4546,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="135.75" hidden="1" thickBot="1">
+    <row r="15" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A15" s="20">
         <v>17</v>
       </c>
@@ -4583,16 +4563,16 @@
         <v>63</v>
       </c>
       <c r="F15" s="23">
-        <v>45033</v>
+        <v>45072</v>
       </c>
       <c r="G15" s="35">
-        <v>45033.721053240741</v>
+        <v>45072.613888888889</v>
       </c>
       <c r="H15" s="38" t="s">
-        <v>325</v>
+        <v>427</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>326</v>
+        <v>428</v>
       </c>
       <c r="J15" s="33" t="s">
         <v>105</v>
@@ -4610,7 +4590,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="135.75" hidden="1" thickBot="1">
+    <row r="16" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A16" s="20">
         <v>18</v>
       </c>
@@ -4627,16 +4607,16 @@
         <v>65</v>
       </c>
       <c r="F16" s="23">
-        <v>45034</v>
+        <v>45072</v>
       </c>
       <c r="G16" s="35">
-        <v>45034.650752314818</v>
+        <v>45072.768217592595</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>335</v>
+        <v>429</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>336</v>
+        <v>430</v>
       </c>
       <c r="J16" s="33" t="s">
         <v>105</v>
@@ -4654,7 +4634,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="135.75" hidden="1" thickBot="1">
+    <row r="17" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A17" s="20">
         <v>19</v>
       </c>
@@ -4671,16 +4651,16 @@
         <v>67</v>
       </c>
       <c r="F17" s="23">
-        <v>45034</v>
+        <v>45075</v>
       </c>
       <c r="G17" s="35">
-        <v>45034.665543981479</v>
+        <v>45075.456226851849</v>
       </c>
       <c r="H17" s="38" t="s">
-        <v>337</v>
+        <v>431</v>
       </c>
       <c r="I17" s="36" t="s">
-        <v>338</v>
+        <v>432</v>
       </c>
       <c r="J17" s="33" t="s">
         <v>105</v>
@@ -4698,7 +4678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="18" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A18" s="20">
         <v>20</v>
       </c>
@@ -4715,16 +4695,16 @@
         <v>69</v>
       </c>
       <c r="F18" s="23">
-        <v>45034</v>
+        <v>45075</v>
       </c>
       <c r="G18" s="35">
-        <v>45034.714479166665</v>
+        <v>45075.547071759262</v>
       </c>
       <c r="H18" s="38" t="s">
-        <v>339</v>
+        <v>433</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>340</v>
+        <v>434</v>
       </c>
       <c r="J18" s="33" t="s">
         <v>105</v>
@@ -4742,7 +4722,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="19" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A19" s="20">
         <v>21</v>
       </c>
@@ -4759,16 +4739,16 @@
         <v>71</v>
       </c>
       <c r="F19" s="23">
-        <v>45034</v>
+        <v>45075</v>
       </c>
       <c r="G19" s="35">
-        <v>45034.729537037034</v>
+        <v>45075.680381944447</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>341</v>
+        <v>435</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>342</v>
+        <v>436</v>
       </c>
       <c r="J19" s="33" t="s">
         <v>105</v>
@@ -4786,7 +4766,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="20" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A20" s="20">
         <v>22</v>
       </c>
@@ -4803,16 +4783,16 @@
         <v>73</v>
       </c>
       <c r="F20" s="23">
-        <v>45034</v>
+        <v>45075</v>
       </c>
       <c r="G20" s="35">
-        <v>45034.75167824074</v>
+        <v>45075.718287037038</v>
       </c>
       <c r="H20" s="38" t="s">
-        <v>343</v>
+        <v>437</v>
       </c>
       <c r="I20" s="36" t="s">
-        <v>344</v>
+        <v>438</v>
       </c>
       <c r="J20" s="33" t="s">
         <v>105</v>
@@ -4830,7 +4810,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="21" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A21" s="20">
         <v>23</v>
       </c>
@@ -4847,16 +4827,16 @@
         <v>75</v>
       </c>
       <c r="F21" s="23">
-        <v>45034</v>
+        <v>45075</v>
       </c>
       <c r="G21" s="35">
-        <v>45034.762800925928</v>
+        <v>45075.738761574074</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>345</v>
+        <v>439</v>
       </c>
       <c r="I21" s="36" t="s">
-        <v>346</v>
+        <v>440</v>
       </c>
       <c r="J21" s="33" t="s">
         <v>105</v>
@@ -4874,7 +4854,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="150.75" thickBot="1">
+    <row r="22" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A22" s="20">
         <v>24</v>
       </c>
@@ -4891,16 +4871,16 @@
         <v>77</v>
       </c>
       <c r="F22" s="23">
-        <v>45015</v>
+        <v>45078</v>
       </c>
       <c r="G22" s="35">
-        <v>45015.712592592594</v>
+        <v>45078.785196759258</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>347</v>
+        <v>447</v>
       </c>
       <c r="I22" s="36" t="s">
-        <v>348</v>
+        <v>448</v>
       </c>
       <c r="J22" s="33" t="s">
         <v>105</v>
@@ -4918,7 +4898,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="150.75" thickBot="1">
+    <row r="23" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A23" s="20">
         <v>25</v>
       </c>
@@ -4935,16 +4915,16 @@
         <v>79</v>
       </c>
       <c r="F23" s="23">
-        <v>45036</v>
+        <v>45079</v>
       </c>
       <c r="G23" s="35">
-        <v>45036.656076388892</v>
+        <v>45079.519467592596</v>
       </c>
       <c r="H23" s="38" t="s">
-        <v>349</v>
+        <v>449</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="J23" s="33" t="s">
         <v>105</v>
@@ -4962,7 +4942,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="150.75" thickBot="1">
+    <row r="24" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A24" s="20">
         <v>26</v>
       </c>
@@ -4978,23 +4958,15 @@
       <c r="E24" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="23">
-        <v>45037</v>
-      </c>
-      <c r="G24" s="35">
-        <v>45037.599317129629</v>
-      </c>
-      <c r="H24" s="38" t="s">
-        <v>352</v>
-      </c>
-      <c r="I24" s="36" t="s">
-        <v>353</v>
-      </c>
+      <c r="F24" s="23"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="36"/>
       <c r="J24" s="33" t="s">
         <v>302</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
@@ -5008,7 +4980,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="150.75" thickBot="1">
+    <row r="25" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A25" s="20">
         <v>27</v>
       </c>
@@ -5024,23 +4996,15 @@
       <c r="E25" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="23">
-        <v>45037</v>
-      </c>
-      <c r="G25" s="35">
-        <v>45037.717083333337</v>
-      </c>
-      <c r="H25" s="38" t="s">
-        <v>354</v>
-      </c>
-      <c r="I25" s="36" t="s">
-        <v>355</v>
-      </c>
+      <c r="F25" s="23"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="36"/>
       <c r="J25" s="33" t="s">
         <v>302</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>351</v>
+        <v>451</v>
       </c>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
@@ -5054,7 +5018,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="26" spans="1:20" ht="145.5" hidden="1" thickBot="1">
       <c r="A26" s="20">
         <v>29</v>
       </c>
@@ -5077,10 +5041,10 @@
         <v>45049.443703703706</v>
       </c>
       <c r="H26" s="36" t="s">
-        <v>373</v>
+        <v>333</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>105</v>
@@ -5093,13 +5057,13 @@
         <v>105</v>
       </c>
       <c r="N26" s="24" t="s">
-        <v>375</v>
+        <v>335</v>
       </c>
       <c r="O26" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P26" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q26" s="24"/>
       <c r="R26" s="25"/>
@@ -5108,7 +5072,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="27" spans="1:20" ht="145.5" thickBot="1">
       <c r="A27" s="20">
         <v>32</v>
       </c>
@@ -5131,10 +5095,10 @@
         <v>45051.682210648149</v>
       </c>
       <c r="H27" s="38" t="s">
-        <v>441</v>
+        <v>401</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>105</v>
@@ -5147,13 +5111,13 @@
         <v>105</v>
       </c>
       <c r="N27" s="24" t="s">
-        <v>375</v>
+        <v>335</v>
       </c>
       <c r="O27" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P27" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q27" s="24"/>
       <c r="R27" s="25"/>
@@ -5162,7 +5126,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="28" spans="1:20" ht="145.5" hidden="1" thickBot="1">
       <c r="A28" s="20">
         <v>33</v>
       </c>
@@ -5185,10 +5149,10 @@
         <v>45049.487303240741</v>
       </c>
       <c r="H28" s="38" t="s">
-        <v>378</v>
+        <v>338</v>
       </c>
       <c r="I28" s="36" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J28" s="33" t="s">
         <v>105</v>
@@ -5201,13 +5165,13 @@
         <v>105</v>
       </c>
       <c r="N28" s="24" t="s">
-        <v>375</v>
+        <v>335</v>
       </c>
       <c r="O28" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P28" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q28" s="24"/>
       <c r="R28" s="25"/>
@@ -5216,7 +5180,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="29" spans="1:20" ht="145.5" hidden="1" thickBot="1">
       <c r="A29" s="20">
         <v>34</v>
       </c>
@@ -5239,10 +5203,10 @@
         <v>45049.728391203702</v>
       </c>
       <c r="H29" s="38" t="s">
-        <v>388</v>
+        <v>348</v>
       </c>
       <c r="I29" s="36" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J29" s="33" t="s">
         <v>105</v>
@@ -5255,13 +5219,13 @@
         <v>105</v>
       </c>
       <c r="N29" s="24" t="s">
-        <v>375</v>
+        <v>335</v>
       </c>
       <c r="O29" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P29" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q29" s="24"/>
       <c r="R29" s="25"/>
@@ -5270,7 +5234,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="150.75" thickBot="1">
+    <row r="30" spans="1:20" ht="145.5" hidden="1" thickBot="1">
       <c r="A30" s="20">
         <v>35</v>
       </c>
@@ -5293,10 +5257,10 @@
         <v>45050.682233796295</v>
       </c>
       <c r="H30" s="38" t="s">
-        <v>404</v>
+        <v>364</v>
       </c>
       <c r="I30" s="36" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J30" s="33" t="s">
         <v>105</v>
@@ -5309,13 +5273,13 @@
         <v>105</v>
       </c>
       <c r="N30" s="24" t="s">
-        <v>375</v>
+        <v>335</v>
       </c>
       <c r="O30" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P30" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q30" s="24"/>
       <c r="R30" s="25"/>
@@ -5324,7 +5288,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="31" spans="1:20" ht="145.5" hidden="1" thickBot="1">
       <c r="A31" s="20">
         <v>37</v>
       </c>
@@ -5347,10 +5311,10 @@
         <v>45049.458009259259</v>
       </c>
       <c r="H31" s="38" t="s">
-        <v>376</v>
+        <v>336</v>
       </c>
       <c r="I31" s="36" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J31" s="33" t="s">
         <v>105</v>
@@ -5363,13 +5327,13 @@
         <v>105</v>
       </c>
       <c r="N31" s="24" t="s">
-        <v>377</v>
+        <v>337</v>
       </c>
       <c r="O31" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P31" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q31" s="24"/>
       <c r="R31" s="25"/>
@@ -5378,7 +5342,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="32" spans="1:20" ht="145.5" thickBot="1">
       <c r="A32" s="20">
         <v>40</v>
       </c>
@@ -5401,10 +5365,10 @@
         <v>45051.703449074077</v>
       </c>
       <c r="H32" s="38" t="s">
-        <v>442</v>
+        <v>402</v>
       </c>
       <c r="I32" s="36" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J32" s="33" t="s">
         <v>105</v>
@@ -5417,13 +5381,13 @@
         <v>105</v>
       </c>
       <c r="N32" s="24" t="s">
-        <v>377</v>
+        <v>337</v>
       </c>
       <c r="O32" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P32" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q32" s="24"/>
       <c r="R32" s="25"/>
@@ -5432,7 +5396,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="33" spans="1:20" ht="145.5" hidden="1" thickBot="1">
       <c r="A33" s="20">
         <v>41</v>
       </c>
@@ -5455,10 +5419,10 @@
         <v>45049.504143518519</v>
       </c>
       <c r="H33" s="38" t="s">
-        <v>379</v>
+        <v>339</v>
       </c>
       <c r="I33" s="36" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J33" s="33" t="s">
         <v>105</v>
@@ -5471,13 +5435,13 @@
         <v>105</v>
       </c>
       <c r="N33" s="24" t="s">
-        <v>377</v>
+        <v>337</v>
       </c>
       <c r="O33" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P33" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q33" s="24"/>
       <c r="R33" s="25"/>
@@ -5486,7 +5450,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="34" spans="1:20" ht="145.5" hidden="1" thickBot="1">
       <c r="A34" s="20">
         <v>42</v>
       </c>
@@ -5509,10 +5473,10 @@
         <v>45050.45894675926</v>
       </c>
       <c r="H34" s="38" t="s">
-        <v>389</v>
+        <v>349</v>
       </c>
       <c r="I34" s="36" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>105</v>
@@ -5525,13 +5489,13 @@
         <v>105</v>
       </c>
       <c r="N34" s="24" t="s">
-        <v>377</v>
+        <v>337</v>
       </c>
       <c r="O34" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P34" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q34" s="24"/>
       <c r="R34" s="25"/>
@@ -5540,7 +5504,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="165.75" thickBot="1">
+    <row r="35" spans="1:20" ht="145.5" hidden="1" thickBot="1">
       <c r="A35" s="20">
         <v>43</v>
       </c>
@@ -5563,10 +5527,10 @@
         <v>45050.726701388892</v>
       </c>
       <c r="H35" s="38" t="s">
-        <v>405</v>
+        <v>365</v>
       </c>
       <c r="I35" s="36" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J35" s="33" t="s">
         <v>105</v>
@@ -5579,13 +5543,13 @@
         <v>105</v>
       </c>
       <c r="N35" s="24" t="s">
-        <v>377</v>
+        <v>337</v>
       </c>
       <c r="O35" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P35" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q35" s="24"/>
       <c r="R35" s="25"/>
@@ -5594,7 +5558,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="195.75" hidden="1" thickBot="1">
+    <row r="36" spans="1:20" ht="160" hidden="1" thickBot="1">
       <c r="A36" s="20">
         <v>45</v>
       </c>
@@ -5621,7 +5585,7 @@
       <c r="N36" s="24"/>
       <c r="O36" s="24"/>
       <c r="P36" s="24" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="Q36" s="24"/>
       <c r="R36" s="25" t="s">
@@ -5632,7 +5596,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="195.75" hidden="1" thickBot="1">
+    <row r="37" spans="1:20" ht="160" thickBot="1">
       <c r="A37" s="20">
         <v>48</v>
       </c>
@@ -5659,7 +5623,7 @@
       <c r="N37" s="24"/>
       <c r="O37" s="24"/>
       <c r="P37" s="24" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="Q37" s="24"/>
       <c r="R37" s="25" t="s">
@@ -5670,7 +5634,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="195.75" hidden="1" thickBot="1">
+    <row r="38" spans="1:20" ht="160" hidden="1" thickBot="1">
       <c r="A38" s="20">
         <v>49</v>
       </c>
@@ -5697,7 +5661,7 @@
       <c r="N38" s="24"/>
       <c r="O38" s="24"/>
       <c r="P38" s="24" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="Q38" s="24"/>
       <c r="R38" s="25" t="s">
@@ -5708,7 +5672,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="195.75" hidden="1" thickBot="1">
+    <row r="39" spans="1:20" ht="160" hidden="1" thickBot="1">
       <c r="A39" s="20">
         <v>50</v>
       </c>
@@ -5735,7 +5699,7 @@
       <c r="N39" s="24"/>
       <c r="O39" s="24"/>
       <c r="P39" s="24" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="Q39" s="24"/>
       <c r="R39" s="25" t="s">
@@ -5746,7 +5710,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="195.75" thickBot="1">
+    <row r="40" spans="1:20" ht="160" hidden="1" thickBot="1">
       <c r="A40" s="20">
         <v>51</v>
       </c>
@@ -5773,7 +5737,7 @@
       <c r="N40" s="24"/>
       <c r="O40" s="24"/>
       <c r="P40" s="24" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="Q40" s="24"/>
       <c r="R40" s="25" t="s">
@@ -5784,7 +5748,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="41" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A41" s="20">
         <v>63</v>
       </c>
@@ -5807,10 +5771,10 @@
         <v>45048.703414351854</v>
       </c>
       <c r="H41" s="38" t="s">
-        <v>370</v>
+        <v>330</v>
       </c>
       <c r="I41" s="36" t="s">
-        <v>371</v>
+        <v>331</v>
       </c>
       <c r="J41" s="33" t="s">
         <v>105</v>
@@ -5823,13 +5787,13 @@
         <v>105</v>
       </c>
       <c r="N41" s="24" t="s">
-        <v>372</v>
+        <v>332</v>
       </c>
       <c r="O41" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P41" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q41" s="24"/>
       <c r="R41" s="25"/>
@@ -5838,7 +5802,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="42" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A42" s="20">
         <v>64</v>
       </c>
@@ -5862,7 +5826,7 @@
         <v>302</v>
       </c>
       <c r="K42" s="33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L42" s="24"/>
       <c r="M42" s="24"/>
@@ -5876,7 +5840,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="43" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A43" s="20">
         <v>65</v>
       </c>
@@ -5900,7 +5864,7 @@
         <v>302</v>
       </c>
       <c r="K43" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L43" s="24"/>
       <c r="M43" s="24"/>
@@ -5914,7 +5878,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="44" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A44" s="20">
         <v>66</v>
       </c>
@@ -5938,7 +5902,7 @@
         <v>302</v>
       </c>
       <c r="K44" s="33" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L44" s="24"/>
       <c r="M44" s="24"/>
@@ -5952,7 +5916,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="45" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A45" s="20">
         <v>67</v>
       </c>
@@ -5976,7 +5940,7 @@
         <v>302</v>
       </c>
       <c r="K45" s="33" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L45" s="24"/>
       <c r="M45" s="24"/>
@@ -5990,7 +5954,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="46" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A46" s="20">
         <v>68</v>
       </c>
@@ -6014,7 +5978,7 @@
         <v>302</v>
       </c>
       <c r="K46" s="33" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L46" s="24"/>
       <c r="M46" s="24"/>
@@ -6028,7 +5992,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="47" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A47" s="20">
         <v>69</v>
       </c>
@@ -6052,7 +6016,7 @@
         <v>302</v>
       </c>
       <c r="K47" s="33" t="s">
-        <v>366</v>
+        <v>326</v>
       </c>
       <c r="L47" s="24"/>
       <c r="M47" s="24"/>
@@ -6066,7 +6030,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="48" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A48" s="20">
         <v>70</v>
       </c>
@@ -6090,7 +6054,7 @@
         <v>302</v>
       </c>
       <c r="K48" s="33" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="L48" s="24"/>
       <c r="M48" s="24"/>
@@ -6104,7 +6068,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="49" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A49" s="20">
         <v>71</v>
       </c>
@@ -6128,7 +6092,7 @@
         <v>302</v>
       </c>
       <c r="K49" s="33" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="L49" s="24"/>
       <c r="M49" s="24"/>
@@ -6142,7 +6106,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="50" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A50" s="20">
         <v>72</v>
       </c>
@@ -6166,7 +6130,7 @@
         <v>302</v>
       </c>
       <c r="K50" s="33" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
@@ -6180,7 +6144,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="51" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A51" s="20">
         <v>73</v>
       </c>
@@ -6203,10 +6167,10 @@
         <v>45048.681261574071</v>
       </c>
       <c r="H51" s="38" t="s">
-        <v>367</v>
+        <v>327</v>
       </c>
       <c r="I51" s="36" t="s">
-        <v>368</v>
+        <v>328</v>
       </c>
       <c r="J51" s="33" t="s">
         <v>105</v>
@@ -6219,13 +6183,13 @@
         <v>105</v>
       </c>
       <c r="N51" s="24" t="s">
-        <v>369</v>
+        <v>329</v>
       </c>
       <c r="O51" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P51" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q51" s="24"/>
       <c r="R51" s="25"/>
@@ -6234,7 +6198,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="52" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A52" s="20">
         <v>74</v>
       </c>
@@ -6258,7 +6222,7 @@
         <v>302</v>
       </c>
       <c r="K52" s="33" t="s">
-        <v>459</v>
+        <v>419</v>
       </c>
       <c r="L52" s="24"/>
       <c r="M52" s="24"/>
@@ -6272,7 +6236,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="135.75" hidden="1" thickBot="1">
+    <row r="53" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A53" s="20">
         <v>94</v>
       </c>
@@ -6296,7 +6260,7 @@
         <v>302</v>
       </c>
       <c r="K53" s="24" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="L53" s="24"/>
       <c r="M53" s="24"/>
@@ -6310,7 +6274,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="135.75" hidden="1" thickBot="1">
+    <row r="54" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A54" s="20">
         <v>95</v>
       </c>
@@ -6334,7 +6298,7 @@
         <v>302</v>
       </c>
       <c r="K54" s="24" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L54" s="24"/>
       <c r="M54" s="24"/>
@@ -6348,7 +6312,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="105.75" hidden="1" thickBot="1">
+    <row r="55" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A55" s="20">
         <v>96</v>
       </c>
@@ -6372,7 +6336,7 @@
         <v>302</v>
       </c>
       <c r="K55" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L55" s="24"/>
       <c r="M55" s="24"/>
@@ -6386,7 +6350,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="56" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A56" s="20">
         <v>97</v>
       </c>
@@ -6410,7 +6374,7 @@
         <v>302</v>
       </c>
       <c r="K56" s="24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L56" s="24"/>
       <c r="M56" s="24"/>
@@ -6424,7 +6388,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="135.75" hidden="1" thickBot="1">
+    <row r="57" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A57" s="20">
         <v>98</v>
       </c>
@@ -6448,7 +6412,7 @@
         <v>302</v>
       </c>
       <c r="K57" s="24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L57" s="24"/>
       <c r="M57" s="24"/>
@@ -6462,7 +6426,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="135.75" hidden="1" thickBot="1">
+    <row r="58" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A58" s="20">
         <v>99</v>
       </c>
@@ -6486,7 +6450,7 @@
         <v>302</v>
       </c>
       <c r="K58" s="24" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L58" s="24"/>
       <c r="M58" s="24"/>
@@ -6500,7 +6464,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="105.75" hidden="1" thickBot="1">
+    <row r="59" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A59" s="20">
         <v>100</v>
       </c>
@@ -6524,7 +6488,7 @@
         <v>302</v>
       </c>
       <c r="K59" s="24" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="L59" s="24"/>
       <c r="M59" s="24"/>
@@ -6538,7 +6502,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="60" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A60" s="20">
         <v>101</v>
       </c>
@@ -6562,7 +6526,7 @@
         <v>302</v>
       </c>
       <c r="K60" s="24" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="L60" s="24"/>
       <c r="M60" s="24"/>
@@ -6576,7 +6540,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="61" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A61" s="20">
         <v>102</v>
       </c>
@@ -6599,10 +6563,10 @@
         <v>45049.579837962963</v>
       </c>
       <c r="H61" s="38" t="s">
-        <v>380</v>
+        <v>340</v>
       </c>
       <c r="I61" s="36" t="s">
-        <v>381</v>
+        <v>341</v>
       </c>
       <c r="J61" s="33" t="s">
         <v>105</v>
@@ -6615,13 +6579,13 @@
         <v>105</v>
       </c>
       <c r="N61" s="24" t="s">
-        <v>426</v>
+        <v>386</v>
       </c>
       <c r="O61" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P61" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q61" s="24"/>
       <c r="R61" s="25"/>
@@ -6630,7 +6594,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="62" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A62" s="20">
         <v>103</v>
       </c>
@@ -6653,10 +6617,10 @@
         <v>45049.612187500003</v>
       </c>
       <c r="H62" s="38" t="s">
-        <v>382</v>
+        <v>342</v>
       </c>
       <c r="I62" s="36" t="s">
-        <v>383</v>
+        <v>343</v>
       </c>
       <c r="J62" s="33" t="s">
         <v>105</v>
@@ -6669,13 +6633,13 @@
         <v>105</v>
       </c>
       <c r="N62" s="24" t="s">
-        <v>384</v>
+        <v>344</v>
       </c>
       <c r="O62" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P62" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q62" s="24"/>
       <c r="R62" s="25"/>
@@ -6684,7 +6648,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="63" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A63" s="20">
         <v>104</v>
       </c>
@@ -6707,10 +6671,10 @@
         <v>45049.641134259262</v>
       </c>
       <c r="H63" s="38" t="s">
-        <v>385</v>
+        <v>345</v>
       </c>
       <c r="I63" s="36" t="s">
-        <v>386</v>
+        <v>346</v>
       </c>
       <c r="J63" s="33" t="s">
         <v>105</v>
@@ -6723,13 +6687,13 @@
         <v>105</v>
       </c>
       <c r="N63" s="24" t="s">
-        <v>387</v>
+        <v>347</v>
       </c>
       <c r="O63" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P63" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q63" s="24"/>
       <c r="R63" s="25"/>
@@ -6738,7 +6702,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="135.75" hidden="1" thickBot="1">
+    <row r="64" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A64" s="20">
         <v>105</v>
       </c>
@@ -6762,7 +6726,7 @@
         <v>302</v>
       </c>
       <c r="K64" s="24" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="L64" s="24"/>
       <c r="M64" s="24"/>
@@ -6776,7 +6740,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="135.75" hidden="1" thickBot="1">
+    <row r="65" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A65" s="20">
         <v>106</v>
       </c>
@@ -6800,7 +6764,7 @@
         <v>302</v>
       </c>
       <c r="K65" s="39" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="L65" s="24"/>
       <c r="M65" s="24"/>
@@ -6814,7 +6778,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="66" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A66" s="20">
         <v>107</v>
       </c>
@@ -6838,7 +6802,7 @@
         <v>302</v>
       </c>
       <c r="K66" s="24" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="L66" s="24"/>
       <c r="M66" s="24"/>
@@ -6852,7 +6816,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="67" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A67" s="20">
         <v>108</v>
       </c>
@@ -6876,7 +6840,7 @@
         <v>302</v>
       </c>
       <c r="K67" s="24" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L67" s="24"/>
       <c r="M67" s="24"/>
@@ -6890,7 +6854,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="68" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A68" s="20">
         <v>109</v>
       </c>
@@ -6914,7 +6878,7 @@
         <v>302</v>
       </c>
       <c r="K68" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L68" s="24"/>
       <c r="M68" s="24"/>
@@ -6928,7 +6892,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="105.75" hidden="1" thickBot="1">
+    <row r="69" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A69" s="20">
         <v>110</v>
       </c>
@@ -6952,7 +6916,7 @@
         <v>302</v>
       </c>
       <c r="K69" s="24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L69" s="24"/>
       <c r="M69" s="24"/>
@@ -6966,7 +6930,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="70" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A70" s="20">
         <v>111</v>
       </c>
@@ -6990,7 +6954,7 @@
         <v>302</v>
       </c>
       <c r="K70" s="24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L70" s="24"/>
       <c r="M70" s="24"/>
@@ -7004,7 +6968,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="71" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A71" s="20">
         <v>112</v>
       </c>
@@ -7028,7 +6992,7 @@
         <v>302</v>
       </c>
       <c r="K71" s="24" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L71" s="24"/>
       <c r="M71" s="24"/>
@@ -7042,7 +7006,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="72" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A72" s="20">
         <v>113</v>
       </c>
@@ -7066,7 +7030,7 @@
         <v>302</v>
       </c>
       <c r="K72" s="24" t="s">
-        <v>390</v>
+        <v>350</v>
       </c>
       <c r="L72" s="24"/>
       <c r="M72" s="24"/>
@@ -7080,7 +7044,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="149.44999999999999" hidden="1" customHeight="1" thickBot="1">
+    <row r="73" spans="1:20" ht="149.5" hidden="1" customHeight="1" thickBot="1">
       <c r="A73" s="20">
         <v>114</v>
       </c>
@@ -7103,10 +7067,10 @@
         <v>45050.579467592594</v>
       </c>
       <c r="H73" s="38" t="s">
-        <v>391</v>
+        <v>351</v>
       </c>
       <c r="I73" s="36" t="s">
-        <v>392</v>
+        <v>352</v>
       </c>
       <c r="J73" s="33" t="s">
         <v>105</v>
@@ -7119,13 +7083,13 @@
         <v>105</v>
       </c>
       <c r="N73" s="24" t="s">
-        <v>393</v>
+        <v>353</v>
       </c>
       <c r="O73" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P73" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q73" s="24"/>
       <c r="R73" s="25"/>
@@ -7158,7 +7122,7 @@
         <v>302</v>
       </c>
       <c r="K74" s="24" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="L74" s="24"/>
       <c r="M74" s="24"/>
@@ -7172,7 +7136,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="75" spans="1:20" ht="145.5" hidden="1" thickBot="1">
       <c r="A75" s="20">
         <v>116</v>
       </c>
@@ -7195,10 +7159,10 @@
         <v>45050.596516203703</v>
       </c>
       <c r="H75" s="38" t="s">
-        <v>394</v>
+        <v>354</v>
       </c>
       <c r="I75" s="36" t="s">
-        <v>395</v>
+        <v>355</v>
       </c>
       <c r="J75" s="33" t="s">
         <v>105</v>
@@ -7211,13 +7175,13 @@
         <v>105</v>
       </c>
       <c r="N75" s="24" t="s">
-        <v>396</v>
+        <v>356</v>
       </c>
       <c r="O75" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P75" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q75" s="24"/>
       <c r="R75" s="25"/>
@@ -7226,7 +7190,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="76" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A76" s="20">
         <v>117</v>
       </c>
@@ -7249,10 +7213,10 @@
         <v>45050.62358796296</v>
       </c>
       <c r="H76" s="38" t="s">
-        <v>397</v>
+        <v>357</v>
       </c>
       <c r="I76" s="36" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="J76" s="33" t="s">
         <v>105</v>
@@ -7265,13 +7229,13 @@
         <v>105</v>
       </c>
       <c r="N76" s="24" t="s">
-        <v>399</v>
+        <v>359</v>
       </c>
       <c r="O76" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P76" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q76" s="24"/>
       <c r="R76" s="25"/>
@@ -7280,7 +7244,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="77" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A77" s="20">
         <v>118</v>
       </c>
@@ -7303,10 +7267,10 @@
         <v>45050.632141203707</v>
       </c>
       <c r="H77" s="38" t="s">
-        <v>400</v>
+        <v>360</v>
       </c>
       <c r="I77" s="36" t="s">
-        <v>401</v>
+        <v>361</v>
       </c>
       <c r="J77" s="33" t="s">
         <v>105</v>
@@ -7319,13 +7283,13 @@
         <v>105</v>
       </c>
       <c r="N77" s="24" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
       <c r="O77" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P77" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q77" s="24"/>
       <c r="R77" s="25"/>
@@ -7334,7 +7298,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="78" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A78" s="20">
         <v>119</v>
       </c>
@@ -7358,7 +7322,7 @@
         <v>302</v>
       </c>
       <c r="K78" s="24" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="L78" s="24"/>
       <c r="M78" s="24"/>
@@ -7372,7 +7336,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="79" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A79" s="20">
         <v>120</v>
       </c>
@@ -7396,7 +7360,7 @@
         <v>302</v>
       </c>
       <c r="K79" s="24" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="L79" s="24"/>
       <c r="M79" s="24"/>
@@ -7410,7 +7374,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="120.75" hidden="1" thickBot="1">
+    <row r="80" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A80" s="20">
         <v>121</v>
       </c>
@@ -7434,7 +7398,7 @@
         <v>302</v>
       </c>
       <c r="K80" s="24" t="s">
-        <v>403</v>
+        <v>363</v>
       </c>
       <c r="L80" s="24"/>
       <c r="M80" s="24"/>
@@ -7448,7 +7412,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="105.75" thickBot="1">
+    <row r="81" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A81" s="20">
         <v>122</v>
       </c>
@@ -7472,7 +7436,7 @@
         <v>302</v>
       </c>
       <c r="K81" s="24" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="L81" s="24"/>
       <c r="M81" s="24"/>
@@ -7486,7 +7450,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="105.75" thickBot="1">
+    <row r="82" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A82" s="20">
         <v>123</v>
       </c>
@@ -7510,7 +7474,7 @@
         <v>302</v>
       </c>
       <c r="K82" s="24" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L82" s="24"/>
       <c r="M82" s="24"/>
@@ -7524,7 +7488,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="105.75" thickBot="1">
+    <row r="83" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A83" s="20">
         <v>124</v>
       </c>
@@ -7548,7 +7512,7 @@
         <v>302</v>
       </c>
       <c r="K83" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L83" s="24"/>
       <c r="M83" s="24"/>
@@ -7562,7 +7526,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="120.75" thickBot="1">
+    <row r="84" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A84" s="20">
         <v>125</v>
       </c>
@@ -7586,7 +7550,7 @@
         <v>302</v>
       </c>
       <c r="K84" s="24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L84" s="24"/>
       <c r="M84" s="24"/>
@@ -7600,7 +7564,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="105.75" thickBot="1">
+    <row r="85" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A85" s="20">
         <v>126</v>
       </c>
@@ -7624,7 +7588,7 @@
         <v>302</v>
       </c>
       <c r="K85" s="24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L85" s="24"/>
       <c r="M85" s="24"/>
@@ -7638,7 +7602,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="105.75" thickBot="1">
+    <row r="86" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A86" s="20">
         <v>127</v>
       </c>
@@ -7662,7 +7626,7 @@
         <v>302</v>
       </c>
       <c r="K86" s="24" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L86" s="24"/>
       <c r="M86" s="24"/>
@@ -7676,7 +7640,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="150.75" thickBot="1">
+    <row r="87" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A87" s="20">
         <v>128</v>
       </c>
@@ -7699,10 +7663,10 @@
         <v>45051.431817129633</v>
       </c>
       <c r="H87" s="38" t="s">
-        <v>406</v>
+        <v>366</v>
       </c>
       <c r="I87" s="36" t="s">
-        <v>407</v>
+        <v>367</v>
       </c>
       <c r="J87" s="33" t="s">
         <v>105</v>
@@ -7715,13 +7679,13 @@
         <v>105</v>
       </c>
       <c r="N87" s="24" t="s">
-        <v>408</v>
+        <v>368</v>
       </c>
       <c r="O87" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P87" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q87" s="24"/>
       <c r="R87" s="25"/>
@@ -7730,7 +7694,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="150.75" thickBot="1">
+    <row r="88" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A88" s="20">
         <v>129</v>
       </c>
@@ -7753,10 +7717,10 @@
         <v>45051.469490740739</v>
       </c>
       <c r="H88" s="38" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="I88" s="36" t="s">
-        <v>410</v>
+        <v>370</v>
       </c>
       <c r="J88" s="33" t="s">
         <v>105</v>
@@ -7769,13 +7733,13 @@
         <v>105</v>
       </c>
       <c r="N88" s="24" t="s">
-        <v>411</v>
+        <v>371</v>
       </c>
       <c r="O88" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P88" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q88" s="24"/>
       <c r="R88" s="25"/>
@@ -7784,7 +7748,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="105.75" thickBot="1">
+    <row r="89" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A89" s="20">
         <v>130</v>
       </c>
@@ -7808,7 +7772,7 @@
         <v>302</v>
       </c>
       <c r="K89" s="24" t="s">
-        <v>412</v>
+        <v>372</v>
       </c>
       <c r="L89" s="24"/>
       <c r="M89" s="24"/>
@@ -7822,7 +7786,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="105.75" thickBot="1">
+    <row r="90" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A90" s="20">
         <v>131</v>
       </c>
@@ -7846,7 +7810,7 @@
         <v>302</v>
       </c>
       <c r="K90" s="24" t="s">
-        <v>413</v>
+        <v>373</v>
       </c>
       <c r="L90" s="24"/>
       <c r="M90" s="24"/>
@@ -7860,7 +7824,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="165.75" thickBot="1">
+    <row r="91" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A91" s="20">
         <v>132</v>
       </c>
@@ -7883,10 +7847,10 @@
         <v>45051.497754629629</v>
       </c>
       <c r="H91" s="38" t="s">
-        <v>414</v>
+        <v>374</v>
       </c>
       <c r="I91" s="36" t="s">
-        <v>415</v>
+        <v>375</v>
       </c>
       <c r="J91" s="33" t="s">
         <v>105</v>
@@ -7899,13 +7863,13 @@
         <v>105</v>
       </c>
       <c r="N91" s="24" t="s">
-        <v>416</v>
+        <v>376</v>
       </c>
       <c r="O91" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P91" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q91" s="24"/>
       <c r="R91" s="25"/>
@@ -7914,7 +7878,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="165.75" thickBot="1">
+    <row r="92" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A92" s="20">
         <v>133</v>
       </c>
@@ -7937,10 +7901,10 @@
         <v>45051.516504629632</v>
       </c>
       <c r="H92" s="38" t="s">
-        <v>417</v>
+        <v>377</v>
       </c>
       <c r="I92" s="36" t="s">
-        <v>418</v>
+        <v>378</v>
       </c>
       <c r="J92" s="33" t="s">
         <v>105</v>
@@ -7953,13 +7917,13 @@
         <v>105</v>
       </c>
       <c r="N92" s="24" t="s">
-        <v>419</v>
+        <v>379</v>
       </c>
       <c r="O92" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P92" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q92" s="24"/>
       <c r="R92" s="25"/>
@@ -7968,7 +7932,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="105.75" thickBot="1">
+    <row r="93" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A93" s="20">
         <v>134</v>
       </c>
@@ -7992,7 +7956,7 @@
         <v>302</v>
       </c>
       <c r="K93" s="24" t="s">
-        <v>420</v>
+        <v>380</v>
       </c>
       <c r="L93" s="24"/>
       <c r="M93" s="24"/>
@@ -8006,7 +7970,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="105.75" thickBot="1">
+    <row r="94" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A94" s="20">
         <v>135</v>
       </c>
@@ -8030,7 +7994,7 @@
         <v>302</v>
       </c>
       <c r="K94" s="24" t="s">
-        <v>420</v>
+        <v>380</v>
       </c>
       <c r="L94" s="24"/>
       <c r="M94" s="24"/>
@@ -8044,7 +8008,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="105.75" thickBot="1">
+    <row r="95" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A95" s="20">
         <v>136</v>
       </c>
@@ -8068,7 +8032,7 @@
         <v>302</v>
       </c>
       <c r="K95" s="24" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="L95" s="24"/>
       <c r="M95" s="24"/>
@@ -8082,7 +8046,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="120.75" thickBot="1">
+    <row r="96" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A96" s="20">
         <v>137</v>
       </c>
@@ -8106,7 +8070,7 @@
         <v>302</v>
       </c>
       <c r="K96" s="24" t="s">
-        <v>422</v>
+        <v>382</v>
       </c>
       <c r="L96" s="24"/>
       <c r="M96" s="24"/>
@@ -8120,7 +8084,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="165.75" thickBot="1">
+    <row r="97" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A97" s="20">
         <v>138</v>
       </c>
@@ -8143,10 +8107,10 @@
         <v>45051.534421296295</v>
       </c>
       <c r="H97" s="38" t="s">
-        <v>423</v>
+        <v>383</v>
       </c>
       <c r="I97" s="36" t="s">
-        <v>424</v>
+        <v>384</v>
       </c>
       <c r="J97" s="33" t="s">
         <v>105</v>
@@ -8159,13 +8123,13 @@
         <v>105</v>
       </c>
       <c r="N97" s="24" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="O97" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P97" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q97" s="24"/>
       <c r="R97" s="25"/>
@@ -8174,7 +8138,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="105.75" thickBot="1">
+    <row r="98" spans="1:20" ht="102" hidden="1" thickBot="1">
       <c r="A98" s="20">
         <v>139</v>
       </c>
@@ -8198,7 +8162,7 @@
         <v>302</v>
       </c>
       <c r="K98" s="24" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="L98" s="24"/>
       <c r="M98" s="24"/>
@@ -8212,7 +8176,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="165.75" thickBot="1">
+    <row r="99" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A99" s="20">
         <v>140</v>
       </c>
@@ -8235,10 +8199,10 @@
         <v>45051.599918981483</v>
       </c>
       <c r="H99" s="38" t="s">
-        <v>428</v>
+        <v>388</v>
       </c>
       <c r="I99" s="36" t="s">
-        <v>429</v>
+        <v>389</v>
       </c>
       <c r="J99" s="33" t="s">
         <v>105</v>
@@ -8251,13 +8215,13 @@
         <v>105</v>
       </c>
       <c r="N99" s="24" t="s">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="O99" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P99" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q99" s="24"/>
       <c r="R99" s="25"/>
@@ -8266,7 +8230,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="120.75" thickBot="1">
+    <row r="100" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A100" s="20">
         <v>141</v>
       </c>
@@ -8290,7 +8254,7 @@
         <v>302</v>
       </c>
       <c r="K100" s="24" t="s">
-        <v>431</v>
+        <v>391</v>
       </c>
       <c r="L100" s="24"/>
       <c r="M100" s="24"/>
@@ -8304,7 +8268,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="165.75" thickBot="1">
+    <row r="101" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A101" s="20">
         <v>142</v>
       </c>
@@ -8327,10 +8291,10 @@
         <v>45051.615173611113</v>
       </c>
       <c r="H101" s="38" t="s">
-        <v>432</v>
+        <v>392</v>
       </c>
       <c r="I101" s="36" t="s">
-        <v>433</v>
+        <v>393</v>
       </c>
       <c r="J101" s="33" t="s">
         <v>105</v>
@@ -8343,13 +8307,13 @@
         <v>105</v>
       </c>
       <c r="N101" s="24" t="s">
-        <v>434</v>
+        <v>394</v>
       </c>
       <c r="O101" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P101" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q101" s="24"/>
       <c r="R101" s="25"/>
@@ -8358,7 +8322,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="165.75" thickBot="1">
+    <row r="102" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A102" s="20">
         <v>143</v>
       </c>
@@ -8381,10 +8345,10 @@
         <v>45051.632314814815</v>
       </c>
       <c r="H102" s="38" t="s">
-        <v>435</v>
+        <v>395</v>
       </c>
       <c r="I102" s="36" t="s">
-        <v>436</v>
+        <v>396</v>
       </c>
       <c r="J102" s="33" t="s">
         <v>105</v>
@@ -8397,13 +8361,13 @@
         <v>105</v>
       </c>
       <c r="N102" s="24" t="s">
-        <v>437</v>
+        <v>397</v>
       </c>
       <c r="O102" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P102" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q102" s="24"/>
       <c r="R102" s="25"/>
@@ -8412,7 +8376,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="165.75" thickBot="1">
+    <row r="103" spans="1:20" ht="131" hidden="1" thickBot="1">
       <c r="A103" s="20">
         <v>144</v>
       </c>
@@ -8435,10 +8399,10 @@
         <v>45051.642523148148</v>
       </c>
       <c r="H103" s="38" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="I103" s="36" t="s">
-        <v>439</v>
+        <v>399</v>
       </c>
       <c r="J103" s="33" t="s">
         <v>105</v>
@@ -8451,13 +8415,13 @@
         <v>105</v>
       </c>
       <c r="N103" s="24" t="s">
-        <v>440</v>
+        <v>400</v>
       </c>
       <c r="O103" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P103" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q103" s="24"/>
       <c r="R103" s="25"/>
@@ -8466,7 +8430,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="120.75" thickBot="1">
+    <row r="104" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A104" s="20">
         <v>145</v>
       </c>
@@ -8490,7 +8454,7 @@
         <v>302</v>
       </c>
       <c r="K104" s="24" t="s">
-        <v>431</v>
+        <v>391</v>
       </c>
       <c r="L104" s="24"/>
       <c r="M104" s="24"/>
@@ -8504,7 +8468,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="120">
+    <row r="105" spans="1:20" ht="116.5" hidden="1" thickBot="1">
       <c r="A105" s="20">
         <v>146</v>
       </c>
@@ -8528,7 +8492,7 @@
         <v>302</v>
       </c>
       <c r="K105" s="24" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="L105" s="24"/>
       <c r="M105" s="24"/>
@@ -8542,7 +8506,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="165" hidden="1">
+    <row r="106" spans="1:20" ht="160" thickBot="1">
       <c r="A106" s="20">
         <v>147</v>
       </c>
@@ -8559,16 +8523,16 @@
         <v>242</v>
       </c>
       <c r="F106" s="23">
-        <v>45042</v>
+        <v>45079</v>
       </c>
       <c r="G106" s="35">
-        <v>45042.607048611113</v>
+        <v>45079.792824074073</v>
       </c>
       <c r="H106" s="38" t="s">
-        <v>356</v>
+        <v>452</v>
       </c>
       <c r="I106" s="36" t="s">
-        <v>357</v>
+        <v>453</v>
       </c>
       <c r="J106" s="33" t="s">
         <v>105</v>
@@ -8586,7 +8550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="165" hidden="1">
+    <row r="107" spans="1:20" ht="160" thickBot="1">
       <c r="A107" s="20">
         <v>148</v>
       </c>
@@ -8602,23 +8566,15 @@
       <c r="E107" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="F107" s="23">
-        <v>45042</v>
-      </c>
-      <c r="G107" s="35">
-        <v>45042.776261574072</v>
-      </c>
-      <c r="H107" s="38" t="s">
-        <v>358</v>
-      </c>
-      <c r="I107" s="36" t="s">
-        <v>359</v>
-      </c>
+      <c r="F107" s="23"/>
+      <c r="G107" s="35"/>
+      <c r="H107" s="38"/>
+      <c r="I107" s="36"/>
       <c r="J107" s="33" t="s">
         <v>302</v>
       </c>
       <c r="K107" s="24" t="s">
-        <v>360</v>
+        <v>324</v>
       </c>
       <c r="L107" s="24"/>
       <c r="M107" s="24"/>
@@ -8632,7 +8588,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="165" hidden="1">
+    <row r="108" spans="1:20" ht="160" thickBot="1">
       <c r="A108" s="20">
         <v>149</v>
       </c>
@@ -8648,23 +8604,15 @@
       <c r="E108" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="F108" s="23">
-        <v>45043</v>
-      </c>
-      <c r="G108" s="35">
-        <v>45043.598506944443</v>
-      </c>
-      <c r="H108" s="38" t="s">
-        <v>361</v>
-      </c>
-      <c r="I108" s="36" t="s">
-        <v>362</v>
-      </c>
+      <c r="F108" s="23"/>
+      <c r="G108" s="35"/>
+      <c r="H108" s="38"/>
+      <c r="I108" s="36"/>
       <c r="J108" s="33" t="s">
         <v>302</v>
       </c>
       <c r="K108" s="24" t="s">
-        <v>363</v>
+        <v>325</v>
       </c>
       <c r="L108" s="24"/>
       <c r="M108" s="24"/>
@@ -8678,7 +8626,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="165" hidden="1">
+    <row r="109" spans="1:20" ht="160" thickBot="1">
       <c r="A109" s="20">
         <v>150</v>
       </c>
@@ -8694,22 +8642,16 @@
       <c r="E109" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="F109" s="23">
-        <v>45043</v>
-      </c>
-      <c r="G109" s="35">
-        <v>45043.66443287037</v>
-      </c>
-      <c r="H109" s="38" t="s">
-        <v>364</v>
-      </c>
-      <c r="I109" s="36" t="s">
-        <v>365</v>
-      </c>
+      <c r="F109" s="23"/>
+      <c r="G109" s="35"/>
+      <c r="H109" s="38"/>
+      <c r="I109" s="36"/>
       <c r="J109" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="K109" s="24"/>
+        <v>302</v>
+      </c>
+      <c r="K109" s="24" t="s">
+        <v>324</v>
+      </c>
       <c r="L109" s="24"/>
       <c r="M109" s="24"/>
       <c r="N109" s="24"/>
@@ -8722,7 +8664,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="120" hidden="1">
+    <row r="110" spans="1:20" ht="102" thickBot="1">
       <c r="A110" s="20">
         <v>151</v>
       </c>
@@ -8746,7 +8688,7 @@
         <v>302</v>
       </c>
       <c r="K110" s="24" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="L110" s="24"/>
       <c r="M110" s="24"/>
@@ -8760,7 +8702,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="135" hidden="1">
+    <row r="111" spans="1:20" ht="116.5" thickBot="1">
       <c r="A111" s="20">
         <v>152</v>
       </c>
@@ -8784,7 +8726,7 @@
         <v>302</v>
       </c>
       <c r="K111" s="24" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L111" s="24"/>
       <c r="M111" s="24"/>
@@ -8798,7 +8740,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="135" hidden="1">
+    <row r="112" spans="1:20" ht="116.5" thickBot="1">
       <c r="A112" s="20">
         <v>153</v>
       </c>
@@ -8822,7 +8764,7 @@
         <v>302</v>
       </c>
       <c r="K112" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L112" s="24"/>
       <c r="M112" s="24"/>
@@ -8836,7 +8778,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="135" hidden="1">
+    <row r="113" spans="1:20" ht="116.5" thickBot="1">
       <c r="A113" s="20">
         <v>154</v>
       </c>
@@ -8860,7 +8802,7 @@
         <v>302</v>
       </c>
       <c r="K113" s="24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L113" s="24"/>
       <c r="M113" s="24"/>
@@ -8874,7 +8816,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="135" hidden="1">
+    <row r="114" spans="1:20" ht="116.5" thickBot="1">
       <c r="A114" s="20">
         <v>155</v>
       </c>
@@ -8898,7 +8840,7 @@
         <v>302</v>
       </c>
       <c r="K114" s="24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L114" s="24"/>
       <c r="M114" s="24"/>
@@ -8912,7 +8854,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="135" hidden="1">
+    <row r="115" spans="1:20" ht="116.5" thickBot="1">
       <c r="A115" s="20">
         <v>156</v>
       </c>
@@ -8936,7 +8878,7 @@
         <v>302</v>
       </c>
       <c r="K115" s="24" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L115" s="24"/>
       <c r="M115" s="24"/>
@@ -8950,7 +8892,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="135" hidden="1">
+    <row r="116" spans="1:20" ht="116.5" thickBot="1">
       <c r="A116" s="20">
         <v>157</v>
       </c>
@@ -8974,7 +8916,7 @@
         <v>302</v>
       </c>
       <c r="K116" s="24" t="s">
-        <v>443</v>
+        <v>403</v>
       </c>
       <c r="L116" s="24"/>
       <c r="M116" s="24"/>
@@ -8988,7 +8930,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="165" hidden="1">
+    <row r="117" spans="1:20" ht="131" thickBot="1">
       <c r="A117" s="20">
         <v>158</v>
       </c>
@@ -9011,10 +8953,10 @@
         <v>45051.739178240743</v>
       </c>
       <c r="H117" s="40" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
       <c r="I117" s="36" t="s">
-        <v>446</v>
+        <v>406</v>
       </c>
       <c r="J117" s="33" t="s">
         <v>105</v>
@@ -9027,13 +8969,13 @@
         <v>105</v>
       </c>
       <c r="N117" s="24" t="s">
-        <v>445</v>
+        <v>405</v>
       </c>
       <c r="O117" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P117" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q117" s="24"/>
       <c r="R117" s="25"/>
@@ -9042,7 +8984,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="120" hidden="1">
+    <row r="118" spans="1:20" ht="102" thickBot="1">
       <c r="A118" s="20">
         <v>159</v>
       </c>
@@ -9066,7 +9008,7 @@
         <v>302</v>
       </c>
       <c r="K118" s="24" t="s">
-        <v>447</v>
+        <v>407</v>
       </c>
       <c r="L118" s="24"/>
       <c r="M118" s="24"/>
@@ -9080,7 +9022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="165" hidden="1">
+    <row r="119" spans="1:20" ht="131" thickBot="1">
       <c r="A119" s="20">
         <v>160</v>
       </c>
@@ -9103,10 +9045,10 @@
         <v>45051.75072916667</v>
       </c>
       <c r="H119" s="38" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="I119" s="36" t="s">
-        <v>449</v>
+        <v>409</v>
       </c>
       <c r="J119" s="33" t="s">
         <v>105</v>
@@ -9119,13 +9061,13 @@
         <v>105</v>
       </c>
       <c r="N119" s="24" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="O119" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P119" s="24" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="Q119" s="24"/>
       <c r="R119" s="25"/>
@@ -9134,7 +9076,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="135" hidden="1">
+    <row r="120" spans="1:20" ht="116.5" thickBot="1">
       <c r="A120" s="20">
         <v>161</v>
       </c>
@@ -9158,7 +9100,7 @@
         <v>302</v>
       </c>
       <c r="K120" s="24" t="s">
-        <v>451</v>
+        <v>411</v>
       </c>
       <c r="L120" s="24"/>
       <c r="M120" s="24"/>
@@ -9172,7 +9114,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="135" hidden="1">
+    <row r="121" spans="1:20" ht="116.5" thickBot="1">
       <c r="A121" s="20">
         <v>162</v>
       </c>
@@ -9196,7 +9138,7 @@
         <v>302</v>
       </c>
       <c r="K121" s="24" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="L121" s="24"/>
       <c r="M121" s="24"/>
@@ -9210,7 +9152,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="135" hidden="1">
+    <row r="122" spans="1:20" ht="116.5" thickBot="1">
       <c r="A122" s="20">
         <v>163</v>
       </c>
@@ -9234,7 +9176,7 @@
         <v>302</v>
       </c>
       <c r="K122" s="24" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="L122" s="24"/>
       <c r="M122" s="24"/>
@@ -9248,7 +9190,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="135" hidden="1">
+    <row r="123" spans="1:20" ht="116.5" thickBot="1">
       <c r="A123" s="20">
         <v>164</v>
       </c>
@@ -9272,7 +9214,7 @@
         <v>302</v>
       </c>
       <c r="K123" s="24" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="L123" s="24"/>
       <c r="M123" s="24"/>
@@ -9286,7 +9228,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="135" hidden="1">
+    <row r="124" spans="1:20" ht="116.5" thickBot="1">
       <c r="A124" s="20">
         <v>165</v>
       </c>
@@ -9310,7 +9252,7 @@
         <v>302</v>
       </c>
       <c r="K124" s="24" t="s">
-        <v>452</v>
+        <v>412</v>
       </c>
       <c r="L124" s="24"/>
       <c r="M124" s="24"/>
@@ -9324,7 +9266,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="135" hidden="1">
+    <row r="125" spans="1:20" ht="116.5" thickBot="1">
       <c r="A125" s="20">
         <v>166</v>
       </c>
@@ -9348,7 +9290,7 @@
         <v>302</v>
       </c>
       <c r="K125" s="24" t="s">
-        <v>453</v>
+        <v>413</v>
       </c>
       <c r="L125" s="24"/>
       <c r="M125" s="24"/>
@@ -9362,7 +9304,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="135" hidden="1">
+    <row r="126" spans="1:20" ht="116.5" thickBot="1">
       <c r="A126" s="20">
         <v>167</v>
       </c>
@@ -9386,7 +9328,7 @@
         <v>302</v>
       </c>
       <c r="K126" s="24" t="s">
-        <v>454</v>
+        <v>414</v>
       </c>
       <c r="L126" s="24"/>
       <c r="M126" s="24"/>
@@ -9400,7 +9342,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="150" hidden="1">
+    <row r="127" spans="1:20" ht="116.5" thickBot="1">
       <c r="A127" s="20">
         <v>168</v>
       </c>
@@ -9423,10 +9365,10 @@
         <v>45051.783020833333</v>
       </c>
       <c r="H127" s="38" t="s">
-        <v>456</v>
+        <v>416</v>
       </c>
       <c r="I127" s="36" t="s">
-        <v>457</v>
+        <v>417</v>
       </c>
       <c r="J127" s="33" t="s">
         <v>105</v>
@@ -9439,13 +9381,13 @@
         <v>105</v>
       </c>
       <c r="N127" s="24" t="s">
-        <v>458</v>
+        <v>418</v>
       </c>
       <c r="O127" s="24" t="s">
         <v>105</v>
       </c>
       <c r="P127" s="24" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="Q127" s="24"/>
       <c r="R127" s="25"/>
@@ -9454,7 +9396,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="135" hidden="1">
+    <row r="128" spans="1:20" ht="116">
       <c r="A128" s="20">
         <v>169</v>
       </c>
@@ -9478,7 +9420,7 @@
         <v>302</v>
       </c>
       <c r="K128" s="24" t="s">
-        <v>455</v>
+        <v>415</v>
       </c>
       <c r="L128" s="24"/>
       <c r="M128" s="24"/>
@@ -19092,7 +19034,7 @@
   <autoFilter ref="A9:T128">
     <filterColumn colId="2">
       <filters>
-        <filter val="VPS"/>
+        <filter val="RSA"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -19125,7 +19067,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'[accreditamento-checklist_V4.2_personalizzato.xlsx]Sheet1'!#REF!</xm:f>
+            <xm:f>[1]Sheet1!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>J10 J26 J44:J50 J42</xm:sqref>
         </x14:dataValidation>
@@ -19144,15 +19086,15 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
     <col min="4" max="4" width="102" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="26" width="8.85546875" customWidth="1"/>
+    <col min="5" max="6" width="8.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" customWidth="1"/>
+    <col min="8" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1">
@@ -19211,7 +19153,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="14.5">
       <c r="A5" s="11" t="s">
         <v>49</v>
       </c>
@@ -19225,7 +19167,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="14.5">
       <c r="A6" s="11" t="s">
         <v>50</v>
       </c>
@@ -20199,11 +20141,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="26" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="3" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>